<commit_message>
update file paths and columns for tableau
</commit_message>
<xml_diff>
--- a/combined-datasets/demographics.xlsx
+++ b/combined-datasets/demographics.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -9118,13 +9118,13 @@
         <v>44018.0</v>
       </c>
       <c r="B449" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C449" t="n">
-        <v>1092.0</v>
+        <v>415.0</v>
       </c>
       <c r="D449" t="n">
-        <v>0.04698390844161432</v>
+        <v>0.01785560623010068</v>
       </c>
       <c r="E449" t="n">
         <v>0.0</v>
@@ -9138,19 +9138,19 @@
         <v>44018.0</v>
       </c>
       <c r="B450" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C450" t="n">
-        <v>4139.0</v>
+        <v>415.0</v>
       </c>
       <c r="D450" t="n">
-        <v>0.17808278117201617</v>
+        <v>0.01785560623010068</v>
       </c>
       <c r="E450" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="F450" t="n">
-        <v>0.0058823529411764705</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="451">
@@ -9158,19 +9158,19 @@
         <v>44018.0</v>
       </c>
       <c r="B451" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C451" t="n">
-        <v>4297.0</v>
+        <v>415.0</v>
       </c>
       <c r="D451" t="n">
-        <v>0.18488081920660873</v>
+        <v>0.01785560623010068</v>
       </c>
       <c r="E451" t="n">
-        <v>11.0</v>
+        <v>0.0</v>
       </c>
       <c r="F451" t="n">
-        <v>0.016176470588235296</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="452">
@@ -9178,19 +9178,19 @@
         <v>44018.0</v>
       </c>
       <c r="B452" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C452" t="n">
-        <v>4179.0</v>
+        <v>1092.0</v>
       </c>
       <c r="D452" t="n">
-        <v>0.17980380345925479</v>
+        <v>0.04698390844161432</v>
       </c>
       <c r="E452" t="n">
-        <v>25.0</v>
+        <v>0.0</v>
       </c>
       <c r="F452" t="n">
-        <v>0.03676470588235294</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="453">
@@ -9198,19 +9198,19 @@
         <v>44018.0</v>
       </c>
       <c r="B453" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C453" t="n">
-        <v>3926.0</v>
+        <v>1092.0</v>
       </c>
       <c r="D453" t="n">
-        <v>0.16891833749247054</v>
+        <v>0.04698390844161432</v>
       </c>
       <c r="E453" t="n">
-        <v>72.0</v>
+        <v>0.0</v>
       </c>
       <c r="F453" t="n">
-        <v>0.10588235294117647</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="454">
@@ -9218,19 +9218,19 @@
         <v>44018.0</v>
       </c>
       <c r="B454" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C454" t="n">
-        <v>1576.0</v>
+        <v>1092.0</v>
       </c>
       <c r="D454" t="n">
-        <v>0.06780827811720162</v>
+        <v>0.04698390844161432</v>
       </c>
       <c r="E454" t="n">
-        <v>70.0</v>
+        <v>0.0</v>
       </c>
       <c r="F454" t="n">
-        <v>0.10294117647058823</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="455">
@@ -9238,19 +9238,19 @@
         <v>44018.0</v>
       </c>
       <c r="B455" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C455" t="n">
-        <v>1145.0</v>
+        <v>1092.0</v>
       </c>
       <c r="D455" t="n">
-        <v>0.04926426297220549</v>
+        <v>0.04698390844161432</v>
       </c>
       <c r="E455" t="n">
-        <v>75.0</v>
+        <v>0.0</v>
       </c>
       <c r="F455" t="n">
-        <v>0.11029411764705882</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="456">
@@ -9258,19 +9258,19 @@
         <v>44018.0</v>
       </c>
       <c r="B456" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C456" t="n">
-        <v>736.0</v>
+        <v>4139.0</v>
       </c>
       <c r="D456" t="n">
-        <v>0.0316668100851906</v>
+        <v>0.17808278117201617</v>
       </c>
       <c r="E456" t="n">
-        <v>71.0</v>
+        <v>4.0</v>
       </c>
       <c r="F456" t="n">
-        <v>0.10441176470588236</v>
+        <v>0.0058823529411764705</v>
       </c>
     </row>
     <row r="457">
@@ -9278,19 +9278,19 @@
         <v>44018.0</v>
       </c>
       <c r="B457" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C457" t="n">
-        <v>560.0</v>
+        <v>4139.0</v>
       </c>
       <c r="D457" t="n">
-        <v>0.024094312021340675</v>
+        <v>0.17808278117201617</v>
       </c>
       <c r="E457" t="n">
-        <v>76.0</v>
+        <v>4.0</v>
       </c>
       <c r="F457" t="n">
-        <v>0.11176470588235295</v>
+        <v>0.0058823529411764705</v>
       </c>
     </row>
     <row r="458">
@@ -9298,19 +9298,19 @@
         <v>44018.0</v>
       </c>
       <c r="B458" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C458" t="n">
-        <v>1068.0</v>
+        <v>4139.0</v>
       </c>
       <c r="D458" t="n">
-        <v>0.04595129506927115</v>
+        <v>0.17808278117201617</v>
       </c>
       <c r="E458" t="n">
-        <v>276.0</v>
+        <v>4.0</v>
       </c>
       <c r="F458" t="n">
-        <v>0.40588235294117647</v>
+        <v>0.0058823529411764705</v>
       </c>
     </row>
     <row r="459">
@@ -9318,19 +9318,19 @@
         <v>44018.0</v>
       </c>
       <c r="B459" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C459" t="n">
-        <v>95.0</v>
+        <v>4139.0</v>
       </c>
       <c r="D459" t="n">
-        <v>0.004087427932191722</v>
+        <v>0.17808278117201617</v>
       </c>
       <c r="E459" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="F459" t="n">
-        <v>0.0</v>
+        <v>0.0058823529411764705</v>
       </c>
     </row>
     <row r="460">
@@ -9338,19 +9338,19 @@
         <v>44018.0</v>
       </c>
       <c r="B460" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C460" t="n">
-        <v>23242.0</v>
+        <v>4297.0</v>
       </c>
       <c r="D460" t="n">
-        <v>1.0</v>
+        <v>0.18488081920660873</v>
       </c>
       <c r="E460" t="n">
-        <v>680.0</v>
+        <v>11.0</v>
       </c>
       <c r="F460" t="n">
-        <v>1.0</v>
+        <v>0.016176470588235296</v>
       </c>
     </row>
     <row r="461">
@@ -9358,18 +9358,858 @@
         <v>44018.0</v>
       </c>
       <c r="B461" t="s">
+        <v>9</v>
+      </c>
+      <c r="C461" t="n">
+        <v>4297.0</v>
+      </c>
+      <c r="D461" t="n">
+        <v>0.18488081920660873</v>
+      </c>
+      <c r="E461" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="F461" t="n">
+        <v>0.016176470588235296</v>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B462" t="s">
+        <v>9</v>
+      </c>
+      <c r="C462" t="n">
+        <v>4297.0</v>
+      </c>
+      <c r="D462" t="n">
+        <v>0.18488081920660873</v>
+      </c>
+      <c r="E462" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="F462" t="n">
+        <v>0.016176470588235296</v>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B463" t="s">
+        <v>9</v>
+      </c>
+      <c r="C463" t="n">
+        <v>4297.0</v>
+      </c>
+      <c r="D463" t="n">
+        <v>0.18488081920660873</v>
+      </c>
+      <c r="E463" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="F463" t="n">
+        <v>0.016176470588235296</v>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B464" t="s">
+        <v>10</v>
+      </c>
+      <c r="C464" t="n">
+        <v>4179.0</v>
+      </c>
+      <c r="D464" t="n">
+        <v>0.17980380345925479</v>
+      </c>
+      <c r="E464" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="F464" t="n">
+        <v>0.03676470588235294</v>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B465" t="s">
+        <v>10</v>
+      </c>
+      <c r="C465" t="n">
+        <v>4179.0</v>
+      </c>
+      <c r="D465" t="n">
+        <v>0.17980380345925479</v>
+      </c>
+      <c r="E465" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="F465" t="n">
+        <v>0.03676470588235294</v>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B466" t="s">
+        <v>10</v>
+      </c>
+      <c r="C466" t="n">
+        <v>4179.0</v>
+      </c>
+      <c r="D466" t="n">
+        <v>0.17980380345925479</v>
+      </c>
+      <c r="E466" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="F466" t="n">
+        <v>0.03676470588235294</v>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B467" t="s">
+        <v>10</v>
+      </c>
+      <c r="C467" t="n">
+        <v>4179.0</v>
+      </c>
+      <c r="D467" t="n">
+        <v>0.17980380345925479</v>
+      </c>
+      <c r="E467" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="F467" t="n">
+        <v>0.03676470588235294</v>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B468" t="s">
+        <v>11</v>
+      </c>
+      <c r="C468" t="n">
+        <v>3926.0</v>
+      </c>
+      <c r="D468" t="n">
+        <v>0.16891833749247054</v>
+      </c>
+      <c r="E468" t="n">
+        <v>72.0</v>
+      </c>
+      <c r="F468" t="n">
+        <v>0.10588235294117647</v>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B469" t="s">
+        <v>11</v>
+      </c>
+      <c r="C469" t="n">
+        <v>3926.0</v>
+      </c>
+      <c r="D469" t="n">
+        <v>0.16891833749247054</v>
+      </c>
+      <c r="E469" t="n">
+        <v>72.0</v>
+      </c>
+      <c r="F469" t="n">
+        <v>0.10588235294117647</v>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B470" t="s">
+        <v>11</v>
+      </c>
+      <c r="C470" t="n">
+        <v>3926.0</v>
+      </c>
+      <c r="D470" t="n">
+        <v>0.16891833749247054</v>
+      </c>
+      <c r="E470" t="n">
+        <v>72.0</v>
+      </c>
+      <c r="F470" t="n">
+        <v>0.10588235294117647</v>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B471" t="s">
+        <v>11</v>
+      </c>
+      <c r="C471" t="n">
+        <v>3926.0</v>
+      </c>
+      <c r="D471" t="n">
+        <v>0.16891833749247054</v>
+      </c>
+      <c r="E471" t="n">
+        <v>72.0</v>
+      </c>
+      <c r="F471" t="n">
+        <v>0.10588235294117647</v>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B472" t="s">
+        <v>12</v>
+      </c>
+      <c r="C472" t="n">
+        <v>1576.0</v>
+      </c>
+      <c r="D472" t="n">
+        <v>0.06780827811720162</v>
+      </c>
+      <c r="E472" t="n">
+        <v>70.0</v>
+      </c>
+      <c r="F472" t="n">
+        <v>0.10294117647058823</v>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B473" t="s">
+        <v>12</v>
+      </c>
+      <c r="C473" t="n">
+        <v>1576.0</v>
+      </c>
+      <c r="D473" t="n">
+        <v>0.06780827811720162</v>
+      </c>
+      <c r="E473" t="n">
+        <v>70.0</v>
+      </c>
+      <c r="F473" t="n">
+        <v>0.10294117647058823</v>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B474" t="s">
+        <v>12</v>
+      </c>
+      <c r="C474" t="n">
+        <v>1576.0</v>
+      </c>
+      <c r="D474" t="n">
+        <v>0.06780827811720162</v>
+      </c>
+      <c r="E474" t="n">
+        <v>70.0</v>
+      </c>
+      <c r="F474" t="n">
+        <v>0.10294117647058823</v>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B475" t="s">
+        <v>12</v>
+      </c>
+      <c r="C475" t="n">
+        <v>1576.0</v>
+      </c>
+      <c r="D475" t="n">
+        <v>0.06780827811720162</v>
+      </c>
+      <c r="E475" t="n">
+        <v>70.0</v>
+      </c>
+      <c r="F475" t="n">
+        <v>0.10294117647058823</v>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B476" t="s">
+        <v>13</v>
+      </c>
+      <c r="C476" t="n">
+        <v>1145.0</v>
+      </c>
+      <c r="D476" t="n">
+        <v>0.04926426297220549</v>
+      </c>
+      <c r="E476" t="n">
+        <v>75.0</v>
+      </c>
+      <c r="F476" t="n">
+        <v>0.11029411764705882</v>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B477" t="s">
+        <v>13</v>
+      </c>
+      <c r="C477" t="n">
+        <v>1145.0</v>
+      </c>
+      <c r="D477" t="n">
+        <v>0.04926426297220549</v>
+      </c>
+      <c r="E477" t="n">
+        <v>75.0</v>
+      </c>
+      <c r="F477" t="n">
+        <v>0.11029411764705882</v>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B478" t="s">
+        <v>13</v>
+      </c>
+      <c r="C478" t="n">
+        <v>1145.0</v>
+      </c>
+      <c r="D478" t="n">
+        <v>0.04926426297220549</v>
+      </c>
+      <c r="E478" t="n">
+        <v>75.0</v>
+      </c>
+      <c r="F478" t="n">
+        <v>0.11029411764705882</v>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B479" t="s">
+        <v>13</v>
+      </c>
+      <c r="C479" t="n">
+        <v>1145.0</v>
+      </c>
+      <c r="D479" t="n">
+        <v>0.04926426297220549</v>
+      </c>
+      <c r="E479" t="n">
+        <v>75.0</v>
+      </c>
+      <c r="F479" t="n">
+        <v>0.11029411764705882</v>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B480" t="s">
+        <v>14</v>
+      </c>
+      <c r="C480" t="n">
+        <v>736.0</v>
+      </c>
+      <c r="D480" t="n">
+        <v>0.0316668100851906</v>
+      </c>
+      <c r="E480" t="n">
+        <v>71.0</v>
+      </c>
+      <c r="F480" t="n">
+        <v>0.10441176470588236</v>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B481" t="s">
+        <v>14</v>
+      </c>
+      <c r="C481" t="n">
+        <v>736.0</v>
+      </c>
+      <c r="D481" t="n">
+        <v>0.0316668100851906</v>
+      </c>
+      <c r="E481" t="n">
+        <v>71.0</v>
+      </c>
+      <c r="F481" t="n">
+        <v>0.10441176470588236</v>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B482" t="s">
+        <v>14</v>
+      </c>
+      <c r="C482" t="n">
+        <v>736.0</v>
+      </c>
+      <c r="D482" t="n">
+        <v>0.0316668100851906</v>
+      </c>
+      <c r="E482" t="n">
+        <v>71.0</v>
+      </c>
+      <c r="F482" t="n">
+        <v>0.10441176470588236</v>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B483" t="s">
+        <v>14</v>
+      </c>
+      <c r="C483" t="n">
+        <v>736.0</v>
+      </c>
+      <c r="D483" t="n">
+        <v>0.0316668100851906</v>
+      </c>
+      <c r="E483" t="n">
+        <v>71.0</v>
+      </c>
+      <c r="F483" t="n">
+        <v>0.10441176470588236</v>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B484" t="s">
+        <v>15</v>
+      </c>
+      <c r="C484" t="n">
+        <v>560.0</v>
+      </c>
+      <c r="D484" t="n">
+        <v>0.024094312021340675</v>
+      </c>
+      <c r="E484" t="n">
+        <v>76.0</v>
+      </c>
+      <c r="F484" t="n">
+        <v>0.11176470588235295</v>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B485" t="s">
+        <v>15</v>
+      </c>
+      <c r="C485" t="n">
+        <v>560.0</v>
+      </c>
+      <c r="D485" t="n">
+        <v>0.024094312021340675</v>
+      </c>
+      <c r="E485" t="n">
+        <v>76.0</v>
+      </c>
+      <c r="F485" t="n">
+        <v>0.11176470588235295</v>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B486" t="s">
+        <v>15</v>
+      </c>
+      <c r="C486" t="n">
+        <v>560.0</v>
+      </c>
+      <c r="D486" t="n">
+        <v>0.024094312021340675</v>
+      </c>
+      <c r="E486" t="n">
+        <v>76.0</v>
+      </c>
+      <c r="F486" t="n">
+        <v>0.11176470588235295</v>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B487" t="s">
+        <v>15</v>
+      </c>
+      <c r="C487" t="n">
+        <v>560.0</v>
+      </c>
+      <c r="D487" t="n">
+        <v>0.024094312021340675</v>
+      </c>
+      <c r="E487" t="n">
+        <v>76.0</v>
+      </c>
+      <c r="F487" t="n">
+        <v>0.11176470588235295</v>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B488" t="s">
+        <v>16</v>
+      </c>
+      <c r="C488" t="n">
+        <v>1068.0</v>
+      </c>
+      <c r="D488" t="n">
+        <v>0.04595129506927115</v>
+      </c>
+      <c r="E488" t="n">
+        <v>276.0</v>
+      </c>
+      <c r="F488" t="n">
+        <v>0.40588235294117647</v>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B489" t="s">
+        <v>16</v>
+      </c>
+      <c r="C489" t="n">
+        <v>1068.0</v>
+      </c>
+      <c r="D489" t="n">
+        <v>0.04595129506927115</v>
+      </c>
+      <c r="E489" t="n">
+        <v>276.0</v>
+      </c>
+      <c r="F489" t="n">
+        <v>0.40588235294117647</v>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B490" t="s">
+        <v>16</v>
+      </c>
+      <c r="C490" t="n">
+        <v>1068.0</v>
+      </c>
+      <c r="D490" t="n">
+        <v>0.04595129506927115</v>
+      </c>
+      <c r="E490" t="n">
+        <v>276.0</v>
+      </c>
+      <c r="F490" t="n">
+        <v>0.40588235294117647</v>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B491" t="s">
+        <v>16</v>
+      </c>
+      <c r="C491" t="n">
+        <v>1068.0</v>
+      </c>
+      <c r="D491" t="n">
+        <v>0.04595129506927115</v>
+      </c>
+      <c r="E491" t="n">
+        <v>276.0</v>
+      </c>
+      <c r="F491" t="n">
+        <v>0.40588235294117647</v>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B492" t="s">
+        <v>17</v>
+      </c>
+      <c r="C492" t="n">
+        <v>95.0</v>
+      </c>
+      <c r="D492" t="n">
+        <v>0.004087427932191722</v>
+      </c>
+      <c r="E492" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F492" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B493" t="s">
+        <v>17</v>
+      </c>
+      <c r="C493" t="n">
+        <v>95.0</v>
+      </c>
+      <c r="D493" t="n">
+        <v>0.004087427932191722</v>
+      </c>
+      <c r="E493" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F493" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B494" t="s">
+        <v>17</v>
+      </c>
+      <c r="C494" t="n">
+        <v>95.0</v>
+      </c>
+      <c r="D494" t="n">
+        <v>0.004087427932191722</v>
+      </c>
+      <c r="E494" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F494" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B495" t="s">
+        <v>17</v>
+      </c>
+      <c r="C495" t="n">
+        <v>95.0</v>
+      </c>
+      <c r="D495" t="n">
+        <v>0.004087427932191722</v>
+      </c>
+      <c r="E495" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F495" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B496" t="s">
+        <v>19</v>
+      </c>
+      <c r="C496" t="n">
+        <v>23242.0</v>
+      </c>
+      <c r="D496" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E496" t="n">
+        <v>680.0</v>
+      </c>
+      <c r="F496" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B497" t="s">
+        <v>19</v>
+      </c>
+      <c r="C497" t="n">
+        <v>23242.0</v>
+      </c>
+      <c r="D497" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E497" t="n">
+        <v>680.0</v>
+      </c>
+      <c r="F497" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B498" t="s">
+        <v>19</v>
+      </c>
+      <c r="C498" t="n">
+        <v>23242.0</v>
+      </c>
+      <c r="D498" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E498" t="n">
+        <v>680.0</v>
+      </c>
+      <c r="F498" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B499" t="s">
+        <v>19</v>
+      </c>
+      <c r="C499" t="n">
+        <v>23242.0</v>
+      </c>
+      <c r="D499" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E499" t="n">
+        <v>680.0</v>
+      </c>
+      <c r="F499" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B500" t="s">
         <v>18</v>
       </c>
-      <c r="C461" t="n">
+      <c r="C500" t="n">
         <v>14.0</v>
       </c>
-      <c r="D461" t="n">
+      <c r="D500" t="n">
         <v>6.02357800533517E-4</v>
       </c>
-      <c r="E461" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F461" t="n">
+      <c r="E500" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F500" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B501" t="s">
+        <v>18</v>
+      </c>
+      <c r="C501" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="D501" t="n">
+        <v>6.02357800533517E-4</v>
+      </c>
+      <c r="E501" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F501" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B502" t="s">
+        <v>18</v>
+      </c>
+      <c r="C502" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="D502" t="n">
+        <v>6.02357800533517E-4</v>
+      </c>
+      <c r="E502" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F502" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="n" s="2">
+        <v>44018.0</v>
+      </c>
+      <c r="B503" t="s">
+        <v>18</v>
+      </c>
+      <c r="C503" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="D503" t="n">
+        <v>6.02357800533517E-4</v>
+      </c>
+      <c r="E503" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F503" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -11551,19 +12391,19 @@
         <v>44018.0</v>
       </c>
       <c r="B109" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C109" t="n">
-        <v>11778.0</v>
+        <v>11250.0</v>
       </c>
       <c r="D109" t="n">
-        <v>0.5067550124774116</v>
+        <v>0.4840375182858618</v>
       </c>
       <c r="E109" t="n">
-        <v>392.0</v>
+        <v>285.0</v>
       </c>
       <c r="F109" t="n">
-        <v>0.5764705882352941</v>
+        <v>0.41911764705882354</v>
       </c>
     </row>
     <row r="110">
@@ -11571,19 +12411,19 @@
         <v>44018.0</v>
       </c>
       <c r="B110" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C110" t="n">
-        <v>23242.0</v>
+        <v>11250.0</v>
       </c>
       <c r="D110" t="n">
-        <v>1.0</v>
+        <v>0.4840375182858618</v>
       </c>
       <c r="E110" t="n">
-        <v>680.0</v>
+        <v>285.0</v>
       </c>
       <c r="F110" t="n">
-        <v>1.0</v>
+        <v>0.41911764705882354</v>
       </c>
     </row>
     <row r="111">
@@ -11591,18 +12431,258 @@
         <v>44018.0</v>
       </c>
       <c r="B111" t="s">
+        <v>20</v>
+      </c>
+      <c r="C111" t="n">
+        <v>11250.0</v>
+      </c>
+      <c r="D111" t="n">
+        <v>0.4840375182858618</v>
+      </c>
+      <c r="E111" t="n">
+        <v>285.0</v>
+      </c>
+      <c r="F111" t="n">
+        <v>0.41911764705882354</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n" s="4">
+        <v>44018.0</v>
+      </c>
+      <c r="B112" t="s">
+        <v>21</v>
+      </c>
+      <c r="C112" t="n">
+        <v>11778.0</v>
+      </c>
+      <c r="D112" t="n">
+        <v>0.5067550124774116</v>
+      </c>
+      <c r="E112" t="n">
+        <v>392.0</v>
+      </c>
+      <c r="F112" t="n">
+        <v>0.5764705882352941</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n" s="4">
+        <v>44018.0</v>
+      </c>
+      <c r="B113" t="s">
+        <v>21</v>
+      </c>
+      <c r="C113" t="n">
+        <v>11778.0</v>
+      </c>
+      <c r="D113" t="n">
+        <v>0.5067550124774116</v>
+      </c>
+      <c r="E113" t="n">
+        <v>392.0</v>
+      </c>
+      <c r="F113" t="n">
+        <v>0.5764705882352941</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n" s="4">
+        <v>44018.0</v>
+      </c>
+      <c r="B114" t="s">
+        <v>21</v>
+      </c>
+      <c r="C114" t="n">
+        <v>11778.0</v>
+      </c>
+      <c r="D114" t="n">
+        <v>0.5067550124774116</v>
+      </c>
+      <c r="E114" t="n">
+        <v>392.0</v>
+      </c>
+      <c r="F114" t="n">
+        <v>0.5764705882352941</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n" s="4">
+        <v>44018.0</v>
+      </c>
+      <c r="B115" t="s">
+        <v>21</v>
+      </c>
+      <c r="C115" t="n">
+        <v>11778.0</v>
+      </c>
+      <c r="D115" t="n">
+        <v>0.5067550124774116</v>
+      </c>
+      <c r="E115" t="n">
+        <v>392.0</v>
+      </c>
+      <c r="F115" t="n">
+        <v>0.5764705882352941</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n" s="4">
+        <v>44018.0</v>
+      </c>
+      <c r="B116" t="s">
+        <v>19</v>
+      </c>
+      <c r="C116" t="n">
+        <v>23242.0</v>
+      </c>
+      <c r="D116" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E116" t="n">
+        <v>680.0</v>
+      </c>
+      <c r="F116" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n" s="4">
+        <v>44018.0</v>
+      </c>
+      <c r="B117" t="s">
+        <v>19</v>
+      </c>
+      <c r="C117" t="n">
+        <v>23242.0</v>
+      </c>
+      <c r="D117" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E117" t="n">
+        <v>680.0</v>
+      </c>
+      <c r="F117" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n" s="4">
+        <v>44018.0</v>
+      </c>
+      <c r="B118" t="s">
+        <v>19</v>
+      </c>
+      <c r="C118" t="n">
+        <v>23242.0</v>
+      </c>
+      <c r="D118" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E118" t="n">
+        <v>680.0</v>
+      </c>
+      <c r="F118" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n" s="4">
+        <v>44018.0</v>
+      </c>
+      <c r="B119" t="s">
+        <v>19</v>
+      </c>
+      <c r="C119" t="n">
+        <v>23242.0</v>
+      </c>
+      <c r="D119" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E119" t="n">
+        <v>680.0</v>
+      </c>
+      <c r="F119" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n" s="4">
+        <v>44018.0</v>
+      </c>
+      <c r="B120" t="s">
         <v>18</v>
       </c>
-      <c r="C111" t="n">
+      <c r="C120" t="n">
         <v>214.0</v>
       </c>
-      <c r="D111" t="n">
+      <c r="D120" t="n">
         <v>0.009207469236726615</v>
       </c>
-      <c r="E111" t="n">
+      <c r="E120" t="n">
         <v>3.0</v>
       </c>
-      <c r="F111" t="n">
+      <c r="F120" t="n">
+        <v>0.004411764705882353</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n" s="4">
+        <v>44018.0</v>
+      </c>
+      <c r="B121" t="s">
+        <v>18</v>
+      </c>
+      <c r="C121" t="n">
+        <v>214.0</v>
+      </c>
+      <c r="D121" t="n">
+        <v>0.009207469236726615</v>
+      </c>
+      <c r="E121" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F121" t="n">
+        <v>0.004411764705882353</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n" s="4">
+        <v>44018.0</v>
+      </c>
+      <c r="B122" t="s">
+        <v>18</v>
+      </c>
+      <c r="C122" t="n">
+        <v>214.0</v>
+      </c>
+      <c r="D122" t="n">
+        <v>0.009207469236726615</v>
+      </c>
+      <c r="E122" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F122" t="n">
+        <v>0.004411764705882353</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n" s="4">
+        <v>44018.0</v>
+      </c>
+      <c r="B123" t="s">
+        <v>18</v>
+      </c>
+      <c r="C123" t="n">
+        <v>214.0</v>
+      </c>
+      <c r="D123" t="n">
+        <v>0.009207469236726615</v>
+      </c>
+      <c r="E123" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F123" t="n">
         <v>0.004411764705882353</v>
       </c>
     </row>
@@ -15824,19 +16904,19 @@
         <v>44018.0</v>
       </c>
       <c r="B211" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C211" t="n">
-        <v>2721.0</v>
+        <v>629.0</v>
       </c>
       <c r="D211" t="n">
-        <v>0.11707254108940711</v>
+        <v>0.027063075466827295</v>
       </c>
       <c r="E211" t="n">
-        <v>87.0</v>
+        <v>14.0</v>
       </c>
       <c r="F211" t="n">
-        <v>0.12794117647058822</v>
+        <v>0.020588235294117647</v>
       </c>
     </row>
     <row r="212">
@@ -15844,19 +16924,19 @@
         <v>44018.0</v>
       </c>
       <c r="B212" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C212" t="n">
-        <v>8907.0</v>
+        <v>629.0</v>
       </c>
       <c r="D212" t="n">
-        <v>0.38322863781085964</v>
+        <v>0.027063075466827295</v>
       </c>
       <c r="E212" t="n">
-        <v>195.0</v>
+        <v>14.0</v>
       </c>
       <c r="F212" t="n">
-        <v>0.2867647058823529</v>
+        <v>0.020588235294117647</v>
       </c>
     </row>
     <row r="213">
@@ -15864,19 +16944,19 @@
         <v>44018.0</v>
       </c>
       <c r="B213" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C213" t="n">
-        <v>121.0</v>
+        <v>629.0</v>
       </c>
       <c r="D213" t="n">
-        <v>0.005206092418896825</v>
+        <v>0.027063075466827295</v>
       </c>
       <c r="E213" t="n">
-        <v>1.0</v>
+        <v>14.0</v>
       </c>
       <c r="F213" t="n">
-        <v>0.0014705882352941176</v>
+        <v>0.020588235294117647</v>
       </c>
     </row>
     <row r="214">
@@ -15884,19 +16964,19 @@
         <v>44018.0</v>
       </c>
       <c r="B214" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C214" t="n">
-        <v>23242.0</v>
+        <v>2721.0</v>
       </c>
       <c r="D214" t="n">
-        <v>1.0</v>
+        <v>0.11707254108940711</v>
       </c>
       <c r="E214" t="n">
-        <v>680.0</v>
+        <v>87.0</v>
       </c>
       <c r="F214" t="n">
-        <v>1.0</v>
+        <v>0.12794117647058822</v>
       </c>
     </row>
     <row r="215">
@@ -15904,19 +16984,19 @@
         <v>44018.0</v>
       </c>
       <c r="B215" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C215" t="n">
-        <v>4939.0</v>
+        <v>2721.0</v>
       </c>
       <c r="D215" t="n">
-        <v>0.21250322691678858</v>
+        <v>0.11707254108940711</v>
       </c>
       <c r="E215" t="n">
-        <v>85.0</v>
+        <v>87.0</v>
       </c>
       <c r="F215" t="n">
-        <v>0.125</v>
+        <v>0.12794117647058822</v>
       </c>
     </row>
     <row r="216">
@@ -15924,18 +17004,438 @@
         <v>44018.0</v>
       </c>
       <c r="B216" t="s">
+        <v>23</v>
+      </c>
+      <c r="C216" t="n">
+        <v>2721.0</v>
+      </c>
+      <c r="D216" t="n">
+        <v>0.11707254108940711</v>
+      </c>
+      <c r="E216" t="n">
+        <v>87.0</v>
+      </c>
+      <c r="F216" t="n">
+        <v>0.12794117647058822</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="n" s="6">
+        <v>44018.0</v>
+      </c>
+      <c r="B217" t="s">
+        <v>23</v>
+      </c>
+      <c r="C217" t="n">
+        <v>2721.0</v>
+      </c>
+      <c r="D217" t="n">
+        <v>0.11707254108940711</v>
+      </c>
+      <c r="E217" t="n">
+        <v>87.0</v>
+      </c>
+      <c r="F217" t="n">
+        <v>0.12794117647058822</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="n" s="6">
+        <v>44018.0</v>
+      </c>
+      <c r="B218" t="s">
+        <v>24</v>
+      </c>
+      <c r="C218" t="n">
+        <v>8907.0</v>
+      </c>
+      <c r="D218" t="n">
+        <v>0.38322863781085964</v>
+      </c>
+      <c r="E218" t="n">
+        <v>195.0</v>
+      </c>
+      <c r="F218" t="n">
+        <v>0.2867647058823529</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="n" s="6">
+        <v>44018.0</v>
+      </c>
+      <c r="B219" t="s">
+        <v>24</v>
+      </c>
+      <c r="C219" t="n">
+        <v>8907.0</v>
+      </c>
+      <c r="D219" t="n">
+        <v>0.38322863781085964</v>
+      </c>
+      <c r="E219" t="n">
+        <v>195.0</v>
+      </c>
+      <c r="F219" t="n">
+        <v>0.2867647058823529</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="n" s="6">
+        <v>44018.0</v>
+      </c>
+      <c r="B220" t="s">
+        <v>24</v>
+      </c>
+      <c r="C220" t="n">
+        <v>8907.0</v>
+      </c>
+      <c r="D220" t="n">
+        <v>0.38322863781085964</v>
+      </c>
+      <c r="E220" t="n">
+        <v>195.0</v>
+      </c>
+      <c r="F220" t="n">
+        <v>0.2867647058823529</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="n" s="6">
+        <v>44018.0</v>
+      </c>
+      <c r="B221" t="s">
+        <v>24</v>
+      </c>
+      <c r="C221" t="n">
+        <v>8907.0</v>
+      </c>
+      <c r="D221" t="n">
+        <v>0.38322863781085964</v>
+      </c>
+      <c r="E221" t="n">
+        <v>195.0</v>
+      </c>
+      <c r="F221" t="n">
+        <v>0.2867647058823529</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="n" s="6">
+        <v>44018.0</v>
+      </c>
+      <c r="B222" t="s">
+        <v>25</v>
+      </c>
+      <c r="C222" t="n">
+        <v>121.0</v>
+      </c>
+      <c r="D222" t="n">
+        <v>0.005206092418896825</v>
+      </c>
+      <c r="E222" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F222" t="n">
+        <v>0.0014705882352941176</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="n" s="6">
+        <v>44018.0</v>
+      </c>
+      <c r="B223" t="s">
+        <v>25</v>
+      </c>
+      <c r="C223" t="n">
+        <v>121.0</v>
+      </c>
+      <c r="D223" t="n">
+        <v>0.005206092418896825</v>
+      </c>
+      <c r="E223" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F223" t="n">
+        <v>0.0014705882352941176</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="n" s="6">
+        <v>44018.0</v>
+      </c>
+      <c r="B224" t="s">
+        <v>25</v>
+      </c>
+      <c r="C224" t="n">
+        <v>121.0</v>
+      </c>
+      <c r="D224" t="n">
+        <v>0.005206092418896825</v>
+      </c>
+      <c r="E224" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F224" t="n">
+        <v>0.0014705882352941176</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="n" s="6">
+        <v>44018.0</v>
+      </c>
+      <c r="B225" t="s">
+        <v>25</v>
+      </c>
+      <c r="C225" t="n">
+        <v>121.0</v>
+      </c>
+      <c r="D225" t="n">
+        <v>0.005206092418896825</v>
+      </c>
+      <c r="E225" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F225" t="n">
+        <v>0.0014705882352941176</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="n" s="6">
+        <v>44018.0</v>
+      </c>
+      <c r="B226" t="s">
+        <v>19</v>
+      </c>
+      <c r="C226" t="n">
+        <v>23242.0</v>
+      </c>
+      <c r="D226" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E226" t="n">
+        <v>680.0</v>
+      </c>
+      <c r="F226" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="n" s="6">
+        <v>44018.0</v>
+      </c>
+      <c r="B227" t="s">
+        <v>19</v>
+      </c>
+      <c r="C227" t="n">
+        <v>23242.0</v>
+      </c>
+      <c r="D227" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E227" t="n">
+        <v>680.0</v>
+      </c>
+      <c r="F227" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="n" s="6">
+        <v>44018.0</v>
+      </c>
+      <c r="B228" t="s">
+        <v>19</v>
+      </c>
+      <c r="C228" t="n">
+        <v>23242.0</v>
+      </c>
+      <c r="D228" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E228" t="n">
+        <v>680.0</v>
+      </c>
+      <c r="F228" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="n" s="6">
+        <v>44018.0</v>
+      </c>
+      <c r="B229" t="s">
+        <v>19</v>
+      </c>
+      <c r="C229" t="n">
+        <v>23242.0</v>
+      </c>
+      <c r="D229" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E229" t="n">
+        <v>680.0</v>
+      </c>
+      <c r="F229" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="n" s="6">
+        <v>44018.0</v>
+      </c>
+      <c r="B230" t="s">
+        <v>18</v>
+      </c>
+      <c r="C230" t="n">
+        <v>4939.0</v>
+      </c>
+      <c r="D230" t="n">
+        <v>0.21250322691678858</v>
+      </c>
+      <c r="E230" t="n">
+        <v>85.0</v>
+      </c>
+      <c r="F230" t="n">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="n" s="6">
+        <v>44018.0</v>
+      </c>
+      <c r="B231" t="s">
+        <v>18</v>
+      </c>
+      <c r="C231" t="n">
+        <v>4939.0</v>
+      </c>
+      <c r="D231" t="n">
+        <v>0.21250322691678858</v>
+      </c>
+      <c r="E231" t="n">
+        <v>85.0</v>
+      </c>
+      <c r="F231" t="n">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="n" s="6">
+        <v>44018.0</v>
+      </c>
+      <c r="B232" t="s">
+        <v>18</v>
+      </c>
+      <c r="C232" t="n">
+        <v>4939.0</v>
+      </c>
+      <c r="D232" t="n">
+        <v>0.21250322691678858</v>
+      </c>
+      <c r="E232" t="n">
+        <v>85.0</v>
+      </c>
+      <c r="F232" t="n">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="n" s="6">
+        <v>44018.0</v>
+      </c>
+      <c r="B233" t="s">
+        <v>18</v>
+      </c>
+      <c r="C233" t="n">
+        <v>4939.0</v>
+      </c>
+      <c r="D233" t="n">
+        <v>0.21250322691678858</v>
+      </c>
+      <c r="E233" t="n">
+        <v>85.0</v>
+      </c>
+      <c r="F233" t="n">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="n" s="6">
+        <v>44018.0</v>
+      </c>
+      <c r="B234" t="s">
         <v>26</v>
       </c>
-      <c r="C216" t="n">
+      <c r="C234" t="n">
         <v>5925.0</v>
       </c>
-      <c r="D216" t="n">
+      <c r="D234" t="n">
         <v>0.25492642629722057</v>
       </c>
-      <c r="E216" t="n">
+      <c r="E234" t="n">
         <v>298.0</v>
       </c>
-      <c r="F216" t="n">
+      <c r="F234" t="n">
+        <v>0.43823529411764706</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="n" s="6">
+        <v>44018.0</v>
+      </c>
+      <c r="B235" t="s">
+        <v>26</v>
+      </c>
+      <c r="C235" t="n">
+        <v>5925.0</v>
+      </c>
+      <c r="D235" t="n">
+        <v>0.25492642629722057</v>
+      </c>
+      <c r="E235" t="n">
+        <v>298.0</v>
+      </c>
+      <c r="F235" t="n">
+        <v>0.43823529411764706</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="n" s="6">
+        <v>44018.0</v>
+      </c>
+      <c r="B236" t="s">
+        <v>26</v>
+      </c>
+      <c r="C236" t="n">
+        <v>5925.0</v>
+      </c>
+      <c r="D236" t="n">
+        <v>0.25492642629722057</v>
+      </c>
+      <c r="E236" t="n">
+        <v>298.0</v>
+      </c>
+      <c r="F236" t="n">
+        <v>0.43823529411764706</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="n" s="6">
+        <v>44018.0</v>
+      </c>
+      <c r="B237" t="s">
+        <v>26</v>
+      </c>
+      <c r="C237" t="n">
+        <v>5925.0</v>
+      </c>
+      <c r="D237" t="n">
+        <v>0.25492642629722057</v>
+      </c>
+      <c r="E237" t="n">
+        <v>298.0</v>
+      </c>
+      <c r="F237" t="n">
         <v>0.43823529411764706</v>
       </c>
     </row>

</xml_diff>

<commit_message>
scraping code updates knitted code
</commit_message>
<xml_diff>
--- a/combined-datasets/demographics.xlsx
+++ b/combined-datasets/demographics.xlsx
@@ -14659,19 +14659,19 @@
     </row>
     <row r="548">
       <c r="A548" s="1" t="n">
-        <v>44026</v>
+        <v>44027</v>
       </c>
       <c r="B548" t="s">
         <v>8</v>
       </c>
       <c r="C548" t="n">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="D548" t="n">
-        <v>0.4157514904</v>
+        <v>0.4225030451</v>
       </c>
       <c r="E548" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F548" t="n">
         <v>0</v>
@@ -14685,19 +14685,19 @@
     </row>
     <row r="549">
       <c r="A549" s="1" t="n">
-        <v>44026</v>
+        <v>44027</v>
       </c>
       <c r="B549" t="s">
         <v>9</v>
       </c>
       <c r="C549" t="n">
-        <v>479</v>
+        <v>496</v>
       </c>
       <c r="D549" t="n">
-        <v>1.8787260747</v>
+        <v>1.8879415347</v>
       </c>
       <c r="E549" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="F549" t="n">
         <v>0</v>
@@ -14711,19 +14711,19 @@
     </row>
     <row r="550">
       <c r="A550" s="1" t="n">
-        <v>44026</v>
+        <v>44027</v>
       </c>
       <c r="B550" t="s">
         <v>10</v>
       </c>
       <c r="C550" t="n">
-        <v>1244</v>
+        <v>1293</v>
       </c>
       <c r="D550" t="n">
-        <v>4.8791967367</v>
+        <v>4.921589525</v>
       </c>
       <c r="E550" t="n">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="F550" t="n">
         <v>0</v>
@@ -14737,51 +14737,51 @@
     </row>
     <row r="551">
       <c r="A551" s="1" t="n">
-        <v>44026</v>
+        <v>44027</v>
       </c>
       <c r="B551" t="s">
         <v>11</v>
       </c>
       <c r="C551" t="n">
-        <v>4718</v>
+        <v>4901</v>
       </c>
       <c r="D551" t="n">
-        <v>18.504863508</v>
+        <v>18.654841657</v>
       </c>
       <c r="E551" t="n">
-        <v>8</v>
+        <v>191</v>
       </c>
       <c r="F551" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G551" t="n">
-        <v>0.6954102921</v>
+        <v>0.5494505495</v>
       </c>
       <c r="H551" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="552">
       <c r="A552" s="1" t="n">
-        <v>44026</v>
+        <v>44027</v>
       </c>
       <c r="B552" t="s">
         <v>12</v>
       </c>
       <c r="C552" t="n">
-        <v>4717</v>
+        <v>4867</v>
       </c>
       <c r="D552" t="n">
-        <v>18.500941324</v>
+        <v>18.525426309</v>
       </c>
       <c r="E552" t="n">
-        <v>10</v>
+        <v>160</v>
       </c>
       <c r="F552" t="n">
         <v>12</v>
       </c>
       <c r="G552" t="n">
-        <v>1.668984701</v>
+        <v>1.6483516484</v>
       </c>
       <c r="H552" t="n">
         <v>0</v>
@@ -14789,51 +14789,51 @@
     </row>
     <row r="553">
       <c r="A553" s="1" t="n">
-        <v>44026</v>
+        <v>44027</v>
       </c>
       <c r="B553" t="s">
         <v>13</v>
       </c>
       <c r="C553" t="n">
-        <v>4538</v>
+        <v>4684</v>
       </c>
       <c r="D553" t="n">
-        <v>17.798870411</v>
+        <v>17.828867235</v>
       </c>
       <c r="E553" t="n">
-        <v>6</v>
+        <v>152</v>
       </c>
       <c r="F553" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G553" t="n">
-        <v>3.6161335188</v>
+        <v>3.8461538462</v>
       </c>
       <c r="H553" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="554">
       <c r="A554" s="1" t="n">
-        <v>44026</v>
+        <v>44027</v>
       </c>
       <c r="B554" t="s">
         <v>14</v>
       </c>
       <c r="C554" t="n">
-        <v>4251</v>
+        <v>4353</v>
       </c>
       <c r="D554" t="n">
-        <v>16.67320364</v>
+        <v>16.568970767</v>
       </c>
       <c r="E554" t="n">
-        <v>7</v>
+        <v>109</v>
       </c>
       <c r="F554" t="n">
         <v>77</v>
       </c>
       <c r="G554" t="n">
-        <v>10.709318498</v>
+        <v>10.576923077</v>
       </c>
       <c r="H554" t="n">
         <v>0</v>
@@ -14841,77 +14841,77 @@
     </row>
     <row r="555">
       <c r="A555" s="1" t="n">
-        <v>44026</v>
+        <v>44027</v>
       </c>
       <c r="B555" t="s">
         <v>15</v>
       </c>
       <c r="C555" t="n">
-        <v>1688</v>
+        <v>1735</v>
       </c>
       <c r="D555" t="n">
-        <v>6.6206463759</v>
+        <v>6.6039890378</v>
       </c>
       <c r="E555" t="n">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="F555" t="n">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G555" t="n">
-        <v>9.8748261474</v>
+        <v>10.164835165</v>
       </c>
       <c r="H555" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="556">
       <c r="A556" s="1" t="n">
-        <v>44026</v>
+        <v>44027</v>
       </c>
       <c r="B556" t="s">
         <v>16</v>
       </c>
       <c r="C556" t="n">
-        <v>1225</v>
+        <v>1266</v>
       </c>
       <c r="D556" t="n">
-        <v>4.8046752432</v>
+        <v>4.818818514</v>
       </c>
       <c r="E556" t="n">
-        <v>-1</v>
+        <v>40</v>
       </c>
       <c r="F556" t="n">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G556" t="n">
-        <v>11.40472879</v>
+        <v>11.538461538</v>
       </c>
       <c r="H556" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="557">
       <c r="A557" s="1" t="n">
-        <v>44026</v>
+        <v>44027</v>
       </c>
       <c r="B557" t="s">
         <v>17</v>
       </c>
       <c r="C557" t="n">
-        <v>795</v>
+        <v>807</v>
       </c>
       <c r="D557" t="n">
-        <v>3.1181361782</v>
+        <v>3.0717113276</v>
       </c>
       <c r="E557" t="n">
-        <v>-1</v>
+        <v>11</v>
       </c>
       <c r="F557" t="n">
         <v>79</v>
       </c>
       <c r="G557" t="n">
-        <v>10.987482615</v>
+        <v>10.851648352</v>
       </c>
       <c r="H557" t="n">
         <v>0</v>
@@ -14919,59 +14919,59 @@
     </row>
     <row r="558">
       <c r="A558" s="1" t="n">
-        <v>44026</v>
+        <v>44027</v>
       </c>
       <c r="B558" t="s">
         <v>18</v>
       </c>
       <c r="C558" t="n">
-        <v>601</v>
+        <v>615</v>
       </c>
       <c r="D558" t="n">
-        <v>2.3572325071</v>
+        <v>2.3408952497</v>
       </c>
       <c r="E558" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F558" t="n">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G558" t="n">
-        <v>11.543810848</v>
+        <v>11.675824176</v>
       </c>
       <c r="H558" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="559">
       <c r="A559" s="1" t="n">
-        <v>44026</v>
+        <v>44027</v>
       </c>
       <c r="B559" t="s">
         <v>19</v>
       </c>
       <c r="C559" t="n">
-        <v>1116</v>
+        <v>1126</v>
       </c>
       <c r="D559" t="n">
-        <v>4.3771572011</v>
+        <v>4.2859317905</v>
       </c>
       <c r="E559" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F559" t="n">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="G559" t="n">
-        <v>39.49930459</v>
+        <v>39.148351648</v>
       </c>
       <c r="H559" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="560">
       <c r="A560" s="1" t="n">
-        <v>44026</v>
+        <v>44027</v>
       </c>
       <c r="B560" t="s">
         <v>20</v>
@@ -14980,7 +14980,7 @@
         <v>18</v>
       </c>
       <c r="D560" t="n">
-        <v>0.0705993097</v>
+        <v>0.0685140073</v>
       </c>
       <c r="E560" t="n">
         <v>0</v>
@@ -18313,77 +18313,77 @@
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
-        <v>44026</v>
+        <v>44027</v>
       </c>
       <c r="B128" t="s">
         <v>21</v>
       </c>
       <c r="C128" t="n">
-        <v>12249</v>
+        <v>12560</v>
       </c>
       <c r="D128" t="n">
-        <v>48.042830248</v>
+        <v>47.807551766</v>
       </c>
       <c r="E128" t="n">
-        <v>22</v>
+        <v>333</v>
       </c>
       <c r="F128" t="n">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="G128" t="n">
-        <v>41.585535466</v>
+        <v>41.208791209</v>
       </c>
       <c r="H128" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
-        <v>44026</v>
+        <v>44027</v>
       </c>
       <c r="B129" t="s">
         <v>22</v>
       </c>
       <c r="C129" t="n">
-        <v>12955</v>
+        <v>13369</v>
       </c>
       <c r="D129" t="n">
-        <v>50.811892062</v>
+        <v>50.886875761</v>
       </c>
       <c r="E129" t="n">
-        <v>10</v>
+        <v>424</v>
       </c>
       <c r="F129" t="n">
-        <v>419</v>
+        <v>427</v>
       </c>
       <c r="G129" t="n">
-        <v>58.275382476</v>
+        <v>58.653846154</v>
       </c>
       <c r="H129" t="n">
-        <v>-1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
-        <v>44026</v>
+        <v>44027</v>
       </c>
       <c r="B130" t="s">
         <v>20</v>
       </c>
       <c r="C130" t="n">
-        <v>292</v>
+        <v>343</v>
       </c>
       <c r="D130" t="n">
-        <v>1.1452776906</v>
+        <v>1.3055724726</v>
       </c>
       <c r="E130" t="n">
-        <v>-1</v>
+        <v>50</v>
       </c>
       <c r="F130" t="n">
         <v>1</v>
       </c>
       <c r="G130" t="n">
-        <v>0.1390820584</v>
+        <v>0.1373626374</v>
       </c>
       <c r="H130" t="n">
         <v>-2</v>
@@ -24827,25 +24827,25 @@
     </row>
     <row r="248">
       <c r="A248" s="1" t="n">
-        <v>44026</v>
+        <v>44027</v>
       </c>
       <c r="B248" t="s">
         <v>23</v>
       </c>
       <c r="C248" t="n">
-        <v>642</v>
+        <v>651</v>
       </c>
       <c r="D248" t="n">
-        <v>2.5180420458</v>
+        <v>2.4779232643</v>
       </c>
       <c r="E248" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F248" t="n">
         <v>14</v>
       </c>
       <c r="G248" t="n">
-        <v>1.9471488178</v>
+        <v>1.9230769231</v>
       </c>
       <c r="H248" t="n">
         <v>0</v>
@@ -24853,77 +24853,77 @@
     </row>
     <row r="249">
       <c r="A249" s="1" t="n">
-        <v>44026</v>
+        <v>44027</v>
       </c>
       <c r="B249" t="s">
         <v>24</v>
       </c>
       <c r="C249" t="n">
-        <v>2916</v>
+        <v>2989</v>
       </c>
       <c r="D249" t="n">
-        <v>11.437088171</v>
+        <v>11.377131547</v>
       </c>
       <c r="E249" t="n">
-        <v>1</v>
+        <v>74</v>
       </c>
       <c r="F249" t="n">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G249" t="n">
-        <v>12.795549374</v>
+        <v>12.912087912</v>
       </c>
       <c r="H249" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="n">
-        <v>44026</v>
+        <v>44027</v>
       </c>
       <c r="B250" t="s">
         <v>25</v>
       </c>
       <c r="C250" t="n">
-        <v>10134</v>
+        <v>10534</v>
       </c>
       <c r="D250" t="n">
-        <v>39.747411359</v>
+        <v>40.09591961</v>
       </c>
       <c r="E250" t="n">
-        <v>24</v>
+        <v>424</v>
       </c>
       <c r="F250" t="n">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G250" t="n">
-        <v>29.207232267</v>
+        <v>28.983516484</v>
       </c>
       <c r="H250" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="n">
-        <v>44026</v>
+        <v>44027</v>
       </c>
       <c r="B251" t="s">
         <v>26</v>
       </c>
       <c r="C251" t="n">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D251" t="n">
-        <v>0.521650455</v>
+        <v>0.5138550548</v>
       </c>
       <c r="E251" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F251" t="n">
         <v>1</v>
       </c>
       <c r="G251" t="n">
-        <v>0.1390820584</v>
+        <v>0.1373626374</v>
       </c>
       <c r="H251" t="n">
         <v>0</v>
@@ -24931,54 +24931,54 @@
     </row>
     <row r="252">
       <c r="A252" s="1" t="n">
-        <v>44026</v>
+        <v>44027</v>
       </c>
       <c r="B252" t="s">
         <v>20</v>
       </c>
       <c r="C252" t="n">
-        <v>5325</v>
+        <v>5441</v>
       </c>
       <c r="D252" t="n">
-        <v>20.885629118</v>
+        <v>20.710261876</v>
       </c>
       <c r="E252" t="n">
-        <v>-2</v>
+        <v>114</v>
       </c>
       <c r="F252" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G252" t="n">
-        <v>12.795549374</v>
+        <v>12.774725275</v>
       </c>
       <c r="H252" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="n">
-        <v>44026</v>
+        <v>44027</v>
       </c>
       <c r="B253" t="s">
         <v>27</v>
       </c>
       <c r="C253" t="n">
-        <v>6346</v>
+        <v>6522</v>
       </c>
       <c r="D253" t="n">
-        <v>24.890178852</v>
+        <v>24.824908648</v>
       </c>
       <c r="E253" t="n">
-        <v>7</v>
+        <v>183</v>
       </c>
       <c r="F253" t="n">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="G253" t="n">
-        <v>43.115438108</v>
+        <v>43.269230769</v>
       </c>
       <c r="H253" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix longitudinal demographic handling & update file
</commit_message>
<xml_diff>
--- a/combined-datasets/demographics.xlsx
+++ b/combined-datasets/demographics.xlsx
@@ -14659,19 +14659,19 @@
     </row>
     <row r="548">
       <c r="A548" s="1" t="n">
-        <v>44027</v>
+        <v>44026</v>
       </c>
       <c r="B548" t="s">
         <v>8</v>
       </c>
       <c r="C548" t="n">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D548" t="n">
-        <v>0.4225030451</v>
+        <v>0.4157514904</v>
       </c>
       <c r="E548" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F548" t="n">
         <v>0</v>
@@ -14685,19 +14685,19 @@
     </row>
     <row r="549">
       <c r="A549" s="1" t="n">
-        <v>44027</v>
+        <v>44026</v>
       </c>
       <c r="B549" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C549" t="n">
-        <v>111</v>
+        <v>479</v>
       </c>
       <c r="D549" t="n">
-        <v>0.4225030451</v>
+        <v>1.8787260747</v>
       </c>
       <c r="E549" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F549" t="n">
         <v>0</v>
@@ -14711,16 +14711,16 @@
     </row>
     <row r="550">
       <c r="A550" s="1" t="n">
-        <v>44027</v>
+        <v>44026</v>
       </c>
       <c r="B550" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C550" t="n">
-        <v>111</v>
+        <v>1244</v>
       </c>
       <c r="D550" t="n">
-        <v>0.4225030451</v>
+        <v>4.8791967367</v>
       </c>
       <c r="E550" t="n">
         <v>0</v>
@@ -14737,25 +14737,25 @@
     </row>
     <row r="551">
       <c r="A551" s="1" t="n">
-        <v>44027</v>
+        <v>44026</v>
       </c>
       <c r="B551" t="s">
+        <v>11</v>
+      </c>
+      <c r="C551" t="n">
+        <v>4718</v>
+      </c>
+      <c r="D551" t="n">
+        <v>18.504863508</v>
+      </c>
+      <c r="E551" t="n">
         <v>8</v>
       </c>
-      <c r="C551" t="n">
-        <v>111</v>
-      </c>
-      <c r="D551" t="n">
-        <v>0.4225030451</v>
-      </c>
-      <c r="E551" t="n">
-        <v>0</v>
-      </c>
       <c r="F551" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G551" t="n">
-        <v>0</v>
+        <v>0.6954102921</v>
       </c>
       <c r="H551" t="n">
         <v>0</v>
@@ -14763,25 +14763,25 @@
     </row>
     <row r="552">
       <c r="A552" s="1" t="n">
-        <v>44027</v>
+        <v>44026</v>
       </c>
       <c r="B552" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C552" t="n">
-        <v>496</v>
+        <v>4717</v>
       </c>
       <c r="D552" t="n">
-        <v>1.8879415347</v>
+        <v>18.500941324</v>
       </c>
       <c r="E552" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F552" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G552" t="n">
-        <v>0</v>
+        <v>1.668984701</v>
       </c>
       <c r="H552" t="n">
         <v>0</v>
@@ -14789,25 +14789,25 @@
     </row>
     <row r="553">
       <c r="A553" s="1" t="n">
-        <v>44027</v>
+        <v>44026</v>
       </c>
       <c r="B553" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C553" t="n">
-        <v>496</v>
+        <v>4538</v>
       </c>
       <c r="D553" t="n">
-        <v>1.8879415347</v>
+        <v>17.798870411</v>
       </c>
       <c r="E553" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F553" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="G553" t="n">
-        <v>0</v>
+        <v>3.6161335188</v>
       </c>
       <c r="H553" t="n">
         <v>0</v>
@@ -14815,25 +14815,25 @@
     </row>
     <row r="554">
       <c r="A554" s="1" t="n">
-        <v>44027</v>
+        <v>44026</v>
       </c>
       <c r="B554" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C554" t="n">
-        <v>496</v>
+        <v>4251</v>
       </c>
       <c r="D554" t="n">
-        <v>1.8879415347</v>
+        <v>16.67320364</v>
       </c>
       <c r="E554" t="n">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F554" t="n">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="G554" t="n">
-        <v>0</v>
+        <v>10.709318498</v>
       </c>
       <c r="H554" t="n">
         <v>0</v>
@@ -14841,51 +14841,51 @@
     </row>
     <row r="555">
       <c r="A555" s="1" t="n">
-        <v>44027</v>
+        <v>44026</v>
       </c>
       <c r="B555" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C555" t="n">
-        <v>496</v>
+        <v>1688</v>
       </c>
       <c r="D555" t="n">
-        <v>1.8879415347</v>
+        <v>6.6206463759</v>
       </c>
       <c r="E555" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="F555" t="n">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="G555" t="n">
-        <v>0</v>
+        <v>9.8748261474</v>
       </c>
       <c r="H555" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="556">
       <c r="A556" s="1" t="n">
-        <v>44027</v>
+        <v>44026</v>
       </c>
       <c r="B556" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C556" t="n">
-        <v>1293</v>
+        <v>1225</v>
       </c>
       <c r="D556" t="n">
-        <v>4.921589525</v>
+        <v>4.8046752432</v>
       </c>
       <c r="E556" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F556" t="n">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="G556" t="n">
-        <v>0</v>
+        <v>11.40472879</v>
       </c>
       <c r="H556" t="n">
         <v>0</v>
@@ -14893,25 +14893,25 @@
     </row>
     <row r="557">
       <c r="A557" s="1" t="n">
-        <v>44027</v>
+        <v>44026</v>
       </c>
       <c r="B557" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C557" t="n">
-        <v>1293</v>
+        <v>795</v>
       </c>
       <c r="D557" t="n">
-        <v>4.921589525</v>
+        <v>3.1181361782</v>
       </c>
       <c r="E557" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F557" t="n">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="G557" t="n">
-        <v>0</v>
+        <v>10.987482615</v>
       </c>
       <c r="H557" t="n">
         <v>0</v>
@@ -14919,25 +14919,25 @@
     </row>
     <row r="558">
       <c r="A558" s="1" t="n">
-        <v>44027</v>
+        <v>44026</v>
       </c>
       <c r="B558" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C558" t="n">
-        <v>1293</v>
+        <v>601</v>
       </c>
       <c r="D558" t="n">
-        <v>4.921589525</v>
+        <v>2.3572325071</v>
       </c>
       <c r="E558" t="n">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="F558" t="n">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="G558" t="n">
-        <v>0</v>
+        <v>11.543810848</v>
       </c>
       <c r="H558" t="n">
         <v>0</v>
@@ -14945,25 +14945,25 @@
     </row>
     <row r="559">
       <c r="A559" s="1" t="n">
-        <v>44027</v>
+        <v>44026</v>
       </c>
       <c r="B559" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C559" t="n">
-        <v>1293</v>
+        <v>1116</v>
       </c>
       <c r="D559" t="n">
-        <v>4.921589525</v>
+        <v>4.3771572011</v>
       </c>
       <c r="E559" t="n">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="F559" t="n">
-        <v>0</v>
+        <v>284</v>
       </c>
       <c r="G559" t="n">
-        <v>0</v>
+        <v>39.49930459</v>
       </c>
       <c r="H559" t="n">
         <v>0</v>
@@ -14971,25 +14971,25 @@
     </row>
     <row r="560">
       <c r="A560" s="1" t="n">
-        <v>44027</v>
+        <v>44026</v>
       </c>
       <c r="B560" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C560" t="n">
-        <v>4901</v>
+        <v>18</v>
       </c>
       <c r="D560" t="n">
-        <v>18.654841657</v>
+        <v>0.0705993097</v>
       </c>
       <c r="E560" t="n">
         <v>0</v>
       </c>
       <c r="F560" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G560" t="n">
-        <v>0.5494505495</v>
+        <v>0</v>
       </c>
       <c r="H560" t="n">
         <v>0</v>
@@ -15000,25 +15000,25 @@
         <v>44027</v>
       </c>
       <c r="B561" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C561" t="n">
-        <v>4901</v>
+        <v>111</v>
       </c>
       <c r="D561" t="n">
-        <v>18.654841657</v>
+        <v>0.4225030451</v>
       </c>
       <c r="E561" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F561" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G561" t="n">
-        <v>0.5494505495</v>
+        <v>0</v>
       </c>
       <c r="H561" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="562">
@@ -15026,22 +15026,22 @@
         <v>44027</v>
       </c>
       <c r="B562" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C562" t="n">
-        <v>4901</v>
+        <v>496</v>
       </c>
       <c r="D562" t="n">
-        <v>18.654841657</v>
+        <v>1.8879415347</v>
       </c>
       <c r="E562" t="n">
-        <v>191</v>
+        <v>17</v>
       </c>
       <c r="F562" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G562" t="n">
-        <v>0.5494505495</v>
+        <v>0</v>
       </c>
       <c r="H562" t="n">
         <v>0</v>
@@ -15052,25 +15052,25 @@
         <v>44027</v>
       </c>
       <c r="B563" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C563" t="n">
-        <v>4901</v>
+        <v>1293</v>
       </c>
       <c r="D563" t="n">
-        <v>18.654841657</v>
+        <v>4.921589525</v>
       </c>
       <c r="E563" t="n">
-        <v>191</v>
+        <v>49</v>
       </c>
       <c r="F563" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G563" t="n">
-        <v>0.5494505495</v>
+        <v>0</v>
       </c>
       <c r="H563" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="564">
@@ -15078,25 +15078,25 @@
         <v>44027</v>
       </c>
       <c r="B564" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C564" t="n">
-        <v>4867</v>
+        <v>4901</v>
       </c>
       <c r="D564" t="n">
-        <v>18.525426309</v>
+        <v>18.654841657</v>
       </c>
       <c r="E564" t="n">
-        <v>160</v>
+        <v>183</v>
       </c>
       <c r="F564" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G564" t="n">
-        <v>1.6483516484</v>
+        <v>0.5494505495</v>
       </c>
       <c r="H564" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="565">
@@ -15113,7 +15113,7 @@
         <v>18.525426309</v>
       </c>
       <c r="E565" t="n">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="F565" t="n">
         <v>12</v>
@@ -15130,25 +15130,25 @@
         <v>44027</v>
       </c>
       <c r="B566" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C566" t="n">
-        <v>4867</v>
+        <v>4684</v>
       </c>
       <c r="D566" t="n">
-        <v>18.525426309</v>
+        <v>17.828867235</v>
       </c>
       <c r="E566" t="n">
-        <v>0</v>
+        <v>146</v>
       </c>
       <c r="F566" t="n">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="G566" t="n">
-        <v>1.6483516484</v>
+        <v>3.8461538462</v>
       </c>
       <c r="H566" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="567">
@@ -15156,22 +15156,22 @@
         <v>44027</v>
       </c>
       <c r="B567" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C567" t="n">
-        <v>4867</v>
+        <v>4353</v>
       </c>
       <c r="D567" t="n">
-        <v>18.525426309</v>
+        <v>16.568970767</v>
       </c>
       <c r="E567" t="n">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="F567" t="n">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="G567" t="n">
-        <v>1.6483516484</v>
+        <v>10.576923077</v>
       </c>
       <c r="H567" t="n">
         <v>0</v>
@@ -15182,25 +15182,25 @@
         <v>44027</v>
       </c>
       <c r="B568" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C568" t="n">
-        <v>4684</v>
+        <v>1735</v>
       </c>
       <c r="D568" t="n">
-        <v>17.828867235</v>
+        <v>6.6039890378</v>
       </c>
       <c r="E568" t="n">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="F568" t="n">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="G568" t="n">
-        <v>3.8461538462</v>
+        <v>10.164835165</v>
       </c>
       <c r="H568" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="569">
@@ -15208,22 +15208,22 @@
         <v>44027</v>
       </c>
       <c r="B569" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C569" t="n">
-        <v>4684</v>
+        <v>1266</v>
       </c>
       <c r="D569" t="n">
-        <v>17.828867235</v>
+        <v>4.818818514</v>
       </c>
       <c r="E569" t="n">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="F569" t="n">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="G569" t="n">
-        <v>3.8461538462</v>
+        <v>11.538461538</v>
       </c>
       <c r="H569" t="n">
         <v>2</v>
@@ -15234,22 +15234,22 @@
         <v>44027</v>
       </c>
       <c r="B570" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C570" t="n">
-        <v>4684</v>
+        <v>807</v>
       </c>
       <c r="D570" t="n">
-        <v>17.828867235</v>
+        <v>3.0717113276</v>
       </c>
       <c r="E570" t="n">
-        <v>152</v>
+        <v>12</v>
       </c>
       <c r="F570" t="n">
-        <v>28</v>
+        <v>79</v>
       </c>
       <c r="G570" t="n">
-        <v>3.8461538462</v>
+        <v>10.851648352</v>
       </c>
       <c r="H570" t="n">
         <v>0</v>
@@ -15260,22 +15260,22 @@
         <v>44027</v>
       </c>
       <c r="B571" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C571" t="n">
-        <v>4684</v>
+        <v>615</v>
       </c>
       <c r="D571" t="n">
-        <v>17.828867235</v>
+        <v>2.3408952497</v>
       </c>
       <c r="E571" t="n">
-        <v>152</v>
+        <v>14</v>
       </c>
       <c r="F571" t="n">
-        <v>28</v>
+        <v>85</v>
       </c>
       <c r="G571" t="n">
-        <v>3.8461538462</v>
+        <v>11.675824176</v>
       </c>
       <c r="H571" t="n">
         <v>2</v>
@@ -15286,25 +15286,25 @@
         <v>44027</v>
       </c>
       <c r="B572" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C572" t="n">
-        <v>4353</v>
+        <v>1126</v>
       </c>
       <c r="D572" t="n">
-        <v>16.568970767</v>
+        <v>4.2859317905</v>
       </c>
       <c r="E572" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F572" t="n">
-        <v>77</v>
+        <v>285</v>
       </c>
       <c r="G572" t="n">
-        <v>10.576923077</v>
+        <v>39.148351648</v>
       </c>
       <c r="H572" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="573">
@@ -15312,22 +15312,22 @@
         <v>44027</v>
       </c>
       <c r="B573" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C573" t="n">
-        <v>4353</v>
+        <v>18</v>
       </c>
       <c r="D573" t="n">
-        <v>16.568970767</v>
+        <v>0.0685140073</v>
       </c>
       <c r="E573" t="n">
         <v>0</v>
       </c>
       <c r="F573" t="n">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="G573" t="n">
-        <v>10.576923077</v>
+        <v>0</v>
       </c>
       <c r="H573" t="n">
         <v>0</v>
@@ -15335,25 +15335,25 @@
     </row>
     <row r="574">
       <c r="A574" s="1" t="n">
-        <v>44027</v>
+        <v>44028</v>
       </c>
       <c r="B574" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C574" t="n">
-        <v>4353</v>
+        <v>117</v>
       </c>
       <c r="D574" t="n">
-        <v>16.568970767</v>
+        <v>0.434298441</v>
       </c>
       <c r="E574" t="n">
-        <v>109</v>
+        <v>6</v>
       </c>
       <c r="F574" t="n">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="G574" t="n">
-        <v>10.576923077</v>
+        <v>0</v>
       </c>
       <c r="H574" t="n">
         <v>0</v>
@@ -15361,25 +15361,25 @@
     </row>
     <row r="575">
       <c r="A575" s="1" t="n">
-        <v>44027</v>
+        <v>44028</v>
       </c>
       <c r="B575" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C575" t="n">
-        <v>4353</v>
+        <v>513</v>
       </c>
       <c r="D575" t="n">
-        <v>16.568970767</v>
+        <v>1.9042316258</v>
       </c>
       <c r="E575" t="n">
-        <v>109</v>
+        <v>17</v>
       </c>
       <c r="F575" t="n">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="G575" t="n">
-        <v>10.576923077</v>
+        <v>0</v>
       </c>
       <c r="H575" t="n">
         <v>0</v>
@@ -15387,25 +15387,25 @@
     </row>
     <row r="576">
       <c r="A576" s="1" t="n">
-        <v>44027</v>
+        <v>44028</v>
       </c>
       <c r="B576" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C576" t="n">
-        <v>1735</v>
+        <v>1343</v>
       </c>
       <c r="D576" t="n">
-        <v>6.6039890378</v>
+        <v>4.9851521901</v>
       </c>
       <c r="E576" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F576" t="n">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="G576" t="n">
-        <v>10.164835165</v>
+        <v>0</v>
       </c>
       <c r="H576" t="n">
         <v>0</v>
@@ -15413,51 +15413,51 @@
     </row>
     <row r="577">
       <c r="A577" s="1" t="n">
-        <v>44027</v>
+        <v>44028</v>
       </c>
       <c r="B577" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C577" t="n">
-        <v>1735</v>
+        <v>5075</v>
       </c>
       <c r="D577" t="n">
-        <v>6.6039890378</v>
+        <v>18.838158872</v>
       </c>
       <c r="E577" t="n">
-        <v>0</v>
+        <v>174</v>
       </c>
       <c r="F577" t="n">
-        <v>74</v>
+        <v>4</v>
       </c>
       <c r="G577" t="n">
-        <v>10.164835165</v>
+        <v>0.5442176871</v>
       </c>
       <c r="H577" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="578">
       <c r="A578" s="1" t="n">
-        <v>44027</v>
+        <v>44028</v>
       </c>
       <c r="B578" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C578" t="n">
-        <v>1735</v>
+        <v>5011</v>
       </c>
       <c r="D578" t="n">
-        <v>6.6039890378</v>
+        <v>18.600593912</v>
       </c>
       <c r="E578" t="n">
-        <v>47</v>
+        <v>144</v>
       </c>
       <c r="F578" t="n">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="G578" t="n">
-        <v>10.164835165</v>
+        <v>1.6326530612</v>
       </c>
       <c r="H578" t="n">
         <v>0</v>
@@ -15465,129 +15465,129 @@
     </row>
     <row r="579">
       <c r="A579" s="1" t="n">
-        <v>44027</v>
+        <v>44028</v>
       </c>
       <c r="B579" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C579" t="n">
-        <v>1735</v>
+        <v>4796</v>
       </c>
       <c r="D579" t="n">
-        <v>6.6039890378</v>
+        <v>17.802524128</v>
       </c>
       <c r="E579" t="n">
-        <v>47</v>
+        <v>112</v>
       </c>
       <c r="F579" t="n">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="G579" t="n">
-        <v>10.164835165</v>
+        <v>3.8095238095</v>
       </c>
       <c r="H579" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="580">
       <c r="A580" s="1" t="n">
-        <v>44027</v>
+        <v>44028</v>
       </c>
       <c r="B580" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C580" t="n">
-        <v>1266</v>
+        <v>4428</v>
       </c>
       <c r="D580" t="n">
-        <v>4.818818514</v>
+        <v>16.436525612</v>
       </c>
       <c r="E580" t="n">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="F580" t="n">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="G580" t="n">
-        <v>11.538461538</v>
+        <v>10.476190476</v>
       </c>
       <c r="H580" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="581">
       <c r="A581" s="1" t="n">
-        <v>44027</v>
+        <v>44028</v>
       </c>
       <c r="B581" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C581" t="n">
-        <v>1266</v>
+        <v>1769</v>
       </c>
       <c r="D581" t="n">
-        <v>4.818818514</v>
+        <v>6.5664439495</v>
       </c>
       <c r="E581" t="n">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F581" t="n">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="G581" t="n">
-        <v>11.538461538</v>
+        <v>10.340136054</v>
       </c>
       <c r="H581" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="582">
       <c r="A582" s="1" t="n">
-        <v>44027</v>
+        <v>44028</v>
       </c>
       <c r="B582" t="s">
         <v>16</v>
       </c>
       <c r="C582" t="n">
-        <v>1266</v>
+        <v>1289</v>
       </c>
       <c r="D582" t="n">
-        <v>4.818818514</v>
+        <v>4.7847067558</v>
       </c>
       <c r="E582" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F582" t="n">
         <v>84</v>
       </c>
       <c r="G582" t="n">
-        <v>11.538461538</v>
+        <v>11.428571429</v>
       </c>
       <c r="H582" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="583">
       <c r="A583" s="1" t="n">
-        <v>44027</v>
+        <v>44028</v>
       </c>
       <c r="B583" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C583" t="n">
-        <v>1266</v>
+        <v>820</v>
       </c>
       <c r="D583" t="n">
-        <v>4.818818514</v>
+        <v>3.0438010393</v>
       </c>
       <c r="E583" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F583" t="n">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G583" t="n">
-        <v>11.538461538</v>
+        <v>10.74829932</v>
       </c>
       <c r="H583" t="n">
         <v>0</v>
@@ -15595,417 +15595,79 @@
     </row>
     <row r="584">
       <c r="A584" s="1" t="n">
-        <v>44027</v>
+        <v>44028</v>
       </c>
       <c r="B584" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C584" t="n">
-        <v>807</v>
+        <v>622</v>
       </c>
       <c r="D584" t="n">
-        <v>3.0717113276</v>
+        <v>2.3088344469</v>
       </c>
       <c r="E584" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F584" t="n">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="G584" t="n">
-        <v>10.851648352</v>
+        <v>11.836734694</v>
       </c>
       <c r="H584" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="585">
       <c r="A585" s="1" t="n">
-        <v>44027</v>
+        <v>44028</v>
       </c>
       <c r="B585" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C585" t="n">
-        <v>807</v>
+        <v>1138</v>
       </c>
       <c r="D585" t="n">
-        <v>3.0717113276</v>
+        <v>4.2242019302</v>
       </c>
       <c r="E585" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F585" t="n">
-        <v>79</v>
+        <v>288</v>
       </c>
       <c r="G585" t="n">
-        <v>10.851648352</v>
+        <v>39.183673469</v>
       </c>
       <c r="H585" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="586">
       <c r="A586" s="1" t="n">
-        <v>44027</v>
+        <v>44028</v>
       </c>
       <c r="B586" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C586" t="n">
-        <v>807</v>
+        <v>19</v>
       </c>
       <c r="D586" t="n">
-        <v>3.0717113276</v>
+        <v>0.0705270973</v>
       </c>
       <c r="E586" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F586" t="n">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="G586" t="n">
-        <v>10.851648352</v>
+        <v>0</v>
       </c>
       <c r="H586" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="587">
-      <c r="A587" s="1" t="n">
-        <v>44027</v>
-      </c>
-      <c r="B587" t="s">
-        <v>17</v>
-      </c>
-      <c r="C587" t="n">
-        <v>807</v>
-      </c>
-      <c r="D587" t="n">
-        <v>3.0717113276</v>
-      </c>
-      <c r="E587" t="n">
-        <v>11</v>
-      </c>
-      <c r="F587" t="n">
-        <v>79</v>
-      </c>
-      <c r="G587" t="n">
-        <v>10.851648352</v>
-      </c>
-      <c r="H587" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="588">
-      <c r="A588" s="1" t="n">
-        <v>44027</v>
-      </c>
-      <c r="B588" t="s">
-        <v>18</v>
-      </c>
-      <c r="C588" t="n">
-        <v>615</v>
-      </c>
-      <c r="D588" t="n">
-        <v>2.3408952497</v>
-      </c>
-      <c r="E588" t="n">
-        <v>0</v>
-      </c>
-      <c r="F588" t="n">
-        <v>85</v>
-      </c>
-      <c r="G588" t="n">
-        <v>11.675824176</v>
-      </c>
-      <c r="H588" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="589">
-      <c r="A589" s="1" t="n">
-        <v>44027</v>
-      </c>
-      <c r="B589" t="s">
-        <v>18</v>
-      </c>
-      <c r="C589" t="n">
-        <v>615</v>
-      </c>
-      <c r="D589" t="n">
-        <v>2.3408952497</v>
-      </c>
-      <c r="E589" t="n">
-        <v>0</v>
-      </c>
-      <c r="F589" t="n">
-        <v>85</v>
-      </c>
-      <c r="G589" t="n">
-        <v>11.675824176</v>
-      </c>
-      <c r="H589" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="590">
-      <c r="A590" s="1" t="n">
-        <v>44027</v>
-      </c>
-      <c r="B590" t="s">
-        <v>18</v>
-      </c>
-      <c r="C590" t="n">
-        <v>615</v>
-      </c>
-      <c r="D590" t="n">
-        <v>2.3408952497</v>
-      </c>
-      <c r="E590" t="n">
-        <v>14</v>
-      </c>
-      <c r="F590" t="n">
-        <v>85</v>
-      </c>
-      <c r="G590" t="n">
-        <v>11.675824176</v>
-      </c>
-      <c r="H590" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="591">
-      <c r="A591" s="1" t="n">
-        <v>44027</v>
-      </c>
-      <c r="B591" t="s">
-        <v>18</v>
-      </c>
-      <c r="C591" t="n">
-        <v>615</v>
-      </c>
-      <c r="D591" t="n">
-        <v>2.3408952497</v>
-      </c>
-      <c r="E591" t="n">
-        <v>14</v>
-      </c>
-      <c r="F591" t="n">
-        <v>85</v>
-      </c>
-      <c r="G591" t="n">
-        <v>11.675824176</v>
-      </c>
-      <c r="H591" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="592">
-      <c r="A592" s="1" t="n">
-        <v>44027</v>
-      </c>
-      <c r="B592" t="s">
-        <v>19</v>
-      </c>
-      <c r="C592" t="n">
-        <v>1126</v>
-      </c>
-      <c r="D592" t="n">
-        <v>4.2859317905</v>
-      </c>
-      <c r="E592" t="n">
-        <v>0</v>
-      </c>
-      <c r="F592" t="n">
-        <v>285</v>
-      </c>
-      <c r="G592" t="n">
-        <v>39.148351648</v>
-      </c>
-      <c r="H592" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="593">
-      <c r="A593" s="1" t="n">
-        <v>44027</v>
-      </c>
-      <c r="B593" t="s">
-        <v>19</v>
-      </c>
-      <c r="C593" t="n">
-        <v>1126</v>
-      </c>
-      <c r="D593" t="n">
-        <v>4.2859317905</v>
-      </c>
-      <c r="E593" t="n">
-        <v>0</v>
-      </c>
-      <c r="F593" t="n">
-        <v>285</v>
-      </c>
-      <c r="G593" t="n">
-        <v>39.148351648</v>
-      </c>
-      <c r="H593" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="594">
-      <c r="A594" s="1" t="n">
-        <v>44027</v>
-      </c>
-      <c r="B594" t="s">
-        <v>19</v>
-      </c>
-      <c r="C594" t="n">
-        <v>1126</v>
-      </c>
-      <c r="D594" t="n">
-        <v>4.2859317905</v>
-      </c>
-      <c r="E594" t="n">
-        <v>10</v>
-      </c>
-      <c r="F594" t="n">
-        <v>285</v>
-      </c>
-      <c r="G594" t="n">
-        <v>39.148351648</v>
-      </c>
-      <c r="H594" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="595">
-      <c r="A595" s="1" t="n">
-        <v>44027</v>
-      </c>
-      <c r="B595" t="s">
-        <v>19</v>
-      </c>
-      <c r="C595" t="n">
-        <v>1126</v>
-      </c>
-      <c r="D595" t="n">
-        <v>4.2859317905</v>
-      </c>
-      <c r="E595" t="n">
-        <v>10</v>
-      </c>
-      <c r="F595" t="n">
-        <v>285</v>
-      </c>
-      <c r="G595" t="n">
-        <v>39.148351648</v>
-      </c>
-      <c r="H595" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="596">
-      <c r="A596" s="1" t="n">
-        <v>44027</v>
-      </c>
-      <c r="B596" t="s">
-        <v>20</v>
-      </c>
-      <c r="C596" t="n">
-        <v>18</v>
-      </c>
-      <c r="D596" t="n">
-        <v>0.0685140073</v>
-      </c>
-      <c r="E596" t="n">
-        <v>0</v>
-      </c>
-      <c r="F596" t="n">
-        <v>0</v>
-      </c>
-      <c r="G596" t="n">
-        <v>0</v>
-      </c>
-      <c r="H596" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="597">
-      <c r="A597" s="1" t="n">
-        <v>44027</v>
-      </c>
-      <c r="B597" t="s">
-        <v>20</v>
-      </c>
-      <c r="C597" t="n">
-        <v>18</v>
-      </c>
-      <c r="D597" t="n">
-        <v>0.0685140073</v>
-      </c>
-      <c r="E597" t="n">
-        <v>0</v>
-      </c>
-      <c r="F597" t="n">
-        <v>0</v>
-      </c>
-      <c r="G597" t="n">
-        <v>0</v>
-      </c>
-      <c r="H597" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="598">
-      <c r="A598" s="1" t="n">
-        <v>44027</v>
-      </c>
-      <c r="B598" t="s">
-        <v>20</v>
-      </c>
-      <c r="C598" t="n">
-        <v>18</v>
-      </c>
-      <c r="D598" t="n">
-        <v>0.0685140073</v>
-      </c>
-      <c r="E598" t="n">
-        <v>0</v>
-      </c>
-      <c r="F598" t="n">
-        <v>0</v>
-      </c>
-      <c r="G598" t="n">
-        <v>0</v>
-      </c>
-      <c r="H598" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="599">
-      <c r="A599" s="1" t="n">
-        <v>44027</v>
-      </c>
-      <c r="B599" t="s">
-        <v>20</v>
-      </c>
-      <c r="C599" t="n">
-        <v>18</v>
-      </c>
-      <c r="D599" t="n">
-        <v>0.0685140073</v>
-      </c>
-      <c r="E599" t="n">
-        <v>0</v>
-      </c>
-      <c r="F599" t="n">
-        <v>0</v>
-      </c>
-      <c r="G599" t="n">
-        <v>0</v>
-      </c>
-      <c r="H599" t="n">
         <v>0</v>
       </c>
     </row>
@@ -19327,80 +18989,80 @@
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
-        <v>44027</v>
+        <v>44026</v>
       </c>
       <c r="B128" t="s">
         <v>21</v>
       </c>
       <c r="C128" t="n">
-        <v>12560</v>
+        <v>12249</v>
       </c>
       <c r="D128" t="n">
-        <v>47.807551766</v>
+        <v>48.042830248</v>
       </c>
       <c r="E128" t="n">
-        <v>333</v>
+        <v>22</v>
       </c>
       <c r="F128" t="n">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G128" t="n">
-        <v>41.208791209</v>
+        <v>41.585535466</v>
       </c>
       <c r="H128" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
-        <v>44027</v>
+        <v>44026</v>
       </c>
       <c r="B129" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C129" t="n">
-        <v>12560</v>
+        <v>12955</v>
       </c>
       <c r="D129" t="n">
-        <v>47.807551766</v>
+        <v>50.811892062</v>
       </c>
       <c r="E129" t="n">
-        <v>333</v>
+        <v>10</v>
       </c>
       <c r="F129" t="n">
-        <v>300</v>
+        <v>419</v>
       </c>
       <c r="G129" t="n">
-        <v>41.208791209</v>
+        <v>58.275382476</v>
       </c>
       <c r="H129" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
-        <v>44027</v>
+        <v>44026</v>
       </c>
       <c r="B130" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C130" t="n">
-        <v>12560</v>
+        <v>292</v>
       </c>
       <c r="D130" t="n">
-        <v>47.807551766</v>
+        <v>1.1452776906</v>
       </c>
       <c r="E130" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F130" t="n">
-        <v>300</v>
+        <v>1</v>
       </c>
       <c r="G130" t="n">
-        <v>41.208791209</v>
+        <v>0.1390820584</v>
       </c>
       <c r="H130" t="n">
-        <v>3</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="131">
@@ -19417,7 +19079,7 @@
         <v>47.807551766</v>
       </c>
       <c r="E131" t="n">
-        <v>0</v>
+        <v>311</v>
       </c>
       <c r="F131" t="n">
         <v>300</v>
@@ -19426,7 +19088,7 @@
         <v>41.208791209</v>
       </c>
       <c r="H131" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132">
@@ -19443,7 +19105,7 @@
         <v>50.886875761</v>
       </c>
       <c r="E132" t="n">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="F132" t="n">
         <v>427</v>
@@ -19452,7 +19114,7 @@
         <v>58.653846154</v>
       </c>
       <c r="H132" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="133">
@@ -19460,22 +19122,22 @@
         <v>44027</v>
       </c>
       <c r="B133" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C133" t="n">
-        <v>13369</v>
+        <v>343</v>
       </c>
       <c r="D133" t="n">
-        <v>50.886875761</v>
+        <v>1.3055724726</v>
       </c>
       <c r="E133" t="n">
-        <v>424</v>
+        <v>51</v>
       </c>
       <c r="F133" t="n">
-        <v>427</v>
+        <v>1</v>
       </c>
       <c r="G133" t="n">
-        <v>58.653846154</v>
+        <v>0.1373626374</v>
       </c>
       <c r="H133" t="n">
         <v>0</v>
@@ -19483,157 +19145,79 @@
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
-        <v>44027</v>
+        <v>44028</v>
       </c>
       <c r="B134" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C134" t="n">
-        <v>13369</v>
+        <v>12852</v>
       </c>
       <c r="D134" t="n">
-        <v>50.886875761</v>
+        <v>47.706013363</v>
       </c>
       <c r="E134" t="n">
-        <v>0</v>
+        <v>292</v>
       </c>
       <c r="F134" t="n">
-        <v>427</v>
+        <v>303</v>
       </c>
       <c r="G134" t="n">
-        <v>58.653846154</v>
+        <v>41.224489796</v>
       </c>
       <c r="H134" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
-        <v>44027</v>
+        <v>44028</v>
       </c>
       <c r="B135" t="s">
         <v>22</v>
       </c>
       <c r="C135" t="n">
-        <v>13369</v>
+        <v>13723</v>
       </c>
       <c r="D135" t="n">
-        <v>50.886875761</v>
+        <v>50.939123979</v>
       </c>
       <c r="E135" t="n">
-        <v>0</v>
+        <v>354</v>
       </c>
       <c r="F135" t="n">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="G135" t="n">
-        <v>58.653846154</v>
+        <v>58.639455782</v>
       </c>
       <c r="H135" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
-        <v>44027</v>
+        <v>44028</v>
       </c>
       <c r="B136" t="s">
         <v>20</v>
       </c>
       <c r="C136" t="n">
-        <v>343</v>
+        <v>365</v>
       </c>
       <c r="D136" t="n">
-        <v>1.3055724726</v>
+        <v>1.3548626578</v>
       </c>
       <c r="E136" t="n">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="F136" t="n">
         <v>1</v>
       </c>
       <c r="G136" t="n">
-        <v>0.1373626374</v>
+        <v>0.1360544218</v>
       </c>
       <c r="H136" t="n">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137" s="1" t="n">
-        <v>44027</v>
-      </c>
-      <c r="B137" t="s">
-        <v>20</v>
-      </c>
-      <c r="C137" t="n">
-        <v>343</v>
-      </c>
-      <c r="D137" t="n">
-        <v>1.3055724726</v>
-      </c>
-      <c r="E137" t="n">
-        <v>50</v>
-      </c>
-      <c r="F137" t="n">
-        <v>1</v>
-      </c>
-      <c r="G137" t="n">
-        <v>0.1373626374</v>
-      </c>
-      <c r="H137" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" s="1" t="n">
-        <v>44027</v>
-      </c>
-      <c r="B138" t="s">
-        <v>20</v>
-      </c>
-      <c r="C138" t="n">
-        <v>343</v>
-      </c>
-      <c r="D138" t="n">
-        <v>1.3055724726</v>
-      </c>
-      <c r="E138" t="n">
-        <v>0</v>
-      </c>
-      <c r="F138" t="n">
-        <v>1</v>
-      </c>
-      <c r="G138" t="n">
-        <v>0.1373626374</v>
-      </c>
-      <c r="H138" t="n">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="139">
-      <c r="A139" s="1" t="n">
-        <v>44027</v>
-      </c>
-      <c r="B139" t="s">
-        <v>20</v>
-      </c>
-      <c r="C139" t="n">
-        <v>343</v>
-      </c>
-      <c r="D139" t="n">
-        <v>1.3055724726</v>
-      </c>
-      <c r="E139" t="n">
-        <v>0</v>
-      </c>
-      <c r="F139" t="n">
-        <v>1</v>
-      </c>
-      <c r="G139" t="n">
-        <v>0.1373626374</v>
-      </c>
-      <c r="H139" t="n">
         <v>0</v>
       </c>
     </row>
@@ -26075,25 +25659,25 @@
     </row>
     <row r="248">
       <c r="A248" s="1" t="n">
-        <v>44027</v>
+        <v>44026</v>
       </c>
       <c r="B248" t="s">
         <v>23</v>
       </c>
       <c r="C248" t="n">
-        <v>651</v>
+        <v>642</v>
       </c>
       <c r="D248" t="n">
-        <v>2.4779232643</v>
+        <v>2.5180420458</v>
       </c>
       <c r="E248" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F248" t="n">
         <v>14</v>
       </c>
       <c r="G248" t="n">
-        <v>1.9230769231</v>
+        <v>1.9471488178</v>
       </c>
       <c r="H248" t="n">
         <v>0</v>
@@ -26101,25 +25685,25 @@
     </row>
     <row r="249">
       <c r="A249" s="1" t="n">
-        <v>44027</v>
+        <v>44026</v>
       </c>
       <c r="B249" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C249" t="n">
-        <v>651</v>
+        <v>2916</v>
       </c>
       <c r="D249" t="n">
-        <v>2.4779232643</v>
+        <v>11.437088171</v>
       </c>
       <c r="E249" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F249" t="n">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="G249" t="n">
-        <v>1.9230769231</v>
+        <v>12.795549374</v>
       </c>
       <c r="H249" t="n">
         <v>0</v>
@@ -26127,25 +25711,25 @@
     </row>
     <row r="250">
       <c r="A250" s="1" t="n">
-        <v>44027</v>
+        <v>44026</v>
       </c>
       <c r="B250" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C250" t="n">
-        <v>651</v>
+        <v>10134</v>
       </c>
       <c r="D250" t="n">
-        <v>2.4779232643</v>
+        <v>39.747411359</v>
       </c>
       <c r="E250" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="F250" t="n">
-        <v>14</v>
+        <v>210</v>
       </c>
       <c r="G250" t="n">
-        <v>1.9230769231</v>
+        <v>29.207232267</v>
       </c>
       <c r="H250" t="n">
         <v>0</v>
@@ -26153,25 +25737,25 @@
     </row>
     <row r="251">
       <c r="A251" s="1" t="n">
-        <v>44027</v>
+        <v>44026</v>
       </c>
       <c r="B251" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C251" t="n">
-        <v>651</v>
+        <v>133</v>
       </c>
       <c r="D251" t="n">
-        <v>2.4779232643</v>
+        <v>0.521650455</v>
       </c>
       <c r="E251" t="n">
         <v>0</v>
       </c>
       <c r="F251" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="G251" t="n">
-        <v>1.9230769231</v>
+        <v>0.1390820584</v>
       </c>
       <c r="H251" t="n">
         <v>0</v>
@@ -26179,51 +25763,51 @@
     </row>
     <row r="252">
       <c r="A252" s="1" t="n">
-        <v>44027</v>
+        <v>44026</v>
       </c>
       <c r="B252" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C252" t="n">
-        <v>2989</v>
+        <v>5325</v>
       </c>
       <c r="D252" t="n">
-        <v>11.377131547</v>
+        <v>20.885629118</v>
       </c>
       <c r="E252" t="n">
-        <v>74</v>
+        <v>-2</v>
       </c>
       <c r="F252" t="n">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G252" t="n">
-        <v>12.912087912</v>
+        <v>12.795549374</v>
       </c>
       <c r="H252" t="n">
-        <v>2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="n">
-        <v>44027</v>
+        <v>44026</v>
       </c>
       <c r="B253" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C253" t="n">
-        <v>2989</v>
+        <v>6346</v>
       </c>
       <c r="D253" t="n">
-        <v>11.377131547</v>
+        <v>24.890178852</v>
       </c>
       <c r="E253" t="n">
-        <v>74</v>
+        <v>7</v>
       </c>
       <c r="F253" t="n">
-        <v>94</v>
+        <v>310</v>
       </c>
       <c r="G253" t="n">
-        <v>12.912087912</v>
+        <v>43.115438108</v>
       </c>
       <c r="H253" t="n">
         <v>0</v>
@@ -26234,25 +25818,25 @@
         <v>44027</v>
       </c>
       <c r="B254" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C254" t="n">
-        <v>2989</v>
+        <v>651</v>
       </c>
       <c r="D254" t="n">
-        <v>11.377131547</v>
+        <v>2.4779232643</v>
       </c>
       <c r="E254" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F254" t="n">
-        <v>94</v>
+        <v>14</v>
       </c>
       <c r="G254" t="n">
-        <v>12.912087912</v>
+        <v>1.9230769231</v>
       </c>
       <c r="H254" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="255">
@@ -26269,7 +25853,7 @@
         <v>11.377131547</v>
       </c>
       <c r="E255" t="n">
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="F255" t="n">
         <v>94</v>
@@ -26278,7 +25862,7 @@
         <v>12.912087912</v>
       </c>
       <c r="H255" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="256">
@@ -26295,7 +25879,7 @@
         <v>40.09591961</v>
       </c>
       <c r="E256" t="n">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="F256" t="n">
         <v>211</v>
@@ -26304,7 +25888,7 @@
         <v>28.983516484</v>
       </c>
       <c r="H256" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="257">
@@ -26312,25 +25896,25 @@
         <v>44027</v>
       </c>
       <c r="B257" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C257" t="n">
-        <v>10534</v>
+        <v>135</v>
       </c>
       <c r="D257" t="n">
-        <v>40.09591961</v>
+        <v>0.5138550548</v>
       </c>
       <c r="E257" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F257" t="n">
-        <v>211</v>
+        <v>1</v>
       </c>
       <c r="G257" t="n">
-        <v>28.983516484</v>
+        <v>0.1373626374</v>
       </c>
       <c r="H257" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="258">
@@ -26338,25 +25922,25 @@
         <v>44027</v>
       </c>
       <c r="B258" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C258" t="n">
-        <v>10534</v>
+        <v>5441</v>
       </c>
       <c r="D258" t="n">
-        <v>40.09591961</v>
+        <v>20.710261876</v>
       </c>
       <c r="E258" t="n">
-        <v>424</v>
+        <v>116</v>
       </c>
       <c r="F258" t="n">
-        <v>211</v>
+        <v>93</v>
       </c>
       <c r="G258" t="n">
-        <v>28.983516484</v>
+        <v>12.774725275</v>
       </c>
       <c r="H258" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="259">
@@ -26364,117 +25948,117 @@
         <v>44027</v>
       </c>
       <c r="B259" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C259" t="n">
-        <v>10534</v>
+        <v>6522</v>
       </c>
       <c r="D259" t="n">
-        <v>40.09591961</v>
+        <v>24.824908648</v>
       </c>
       <c r="E259" t="n">
-        <v>424</v>
+        <v>176</v>
       </c>
       <c r="F259" t="n">
-        <v>211</v>
+        <v>315</v>
       </c>
       <c r="G259" t="n">
-        <v>28.983516484</v>
+        <v>43.269230769</v>
       </c>
       <c r="H259" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="n">
-        <v>44027</v>
+        <v>44028</v>
       </c>
       <c r="B260" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C260" t="n">
-        <v>135</v>
+        <v>654</v>
       </c>
       <c r="D260" t="n">
-        <v>0.5138550548</v>
+        <v>2.4276169265</v>
       </c>
       <c r="E260" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F260" t="n">
+        <v>15</v>
+      </c>
+      <c r="G260" t="n">
+        <v>2.0408163265</v>
+      </c>
+      <c r="H260" t="n">
         <v>1</v>
-      </c>
-      <c r="G260" t="n">
-        <v>0.1373626374</v>
-      </c>
-      <c r="H260" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="n">
-        <v>44027</v>
+        <v>44028</v>
       </c>
       <c r="B261" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C261" t="n">
-        <v>135</v>
+        <v>3061</v>
       </c>
       <c r="D261" t="n">
-        <v>0.5138550548</v>
+        <v>11.362286563</v>
       </c>
       <c r="E261" t="n">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="F261" t="n">
+        <v>95</v>
+      </c>
+      <c r="G261" t="n">
+        <v>12.925170068</v>
+      </c>
+      <c r="H261" t="n">
         <v>1</v>
-      </c>
-      <c r="G261" t="n">
-        <v>0.1373626374</v>
-      </c>
-      <c r="H261" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="n">
-        <v>44027</v>
+        <v>44028</v>
       </c>
       <c r="B262" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C262" t="n">
-        <v>135</v>
+        <v>10891</v>
       </c>
       <c r="D262" t="n">
-        <v>0.5138550548</v>
+        <v>40.426874536</v>
       </c>
       <c r="E262" t="n">
-        <v>2</v>
+        <v>357</v>
       </c>
       <c r="F262" t="n">
-        <v>1</v>
+        <v>214</v>
       </c>
       <c r="G262" t="n">
-        <v>0.1373626374</v>
+        <v>29.115646259</v>
       </c>
       <c r="H262" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="n">
-        <v>44027</v>
+        <v>44028</v>
       </c>
       <c r="B263" t="s">
         <v>26</v>
       </c>
       <c r="C263" t="n">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D263" t="n">
-        <v>0.5138550548</v>
+        <v>0.5085374907</v>
       </c>
       <c r="E263" t="n">
         <v>2</v>
@@ -26483,7 +26067,7 @@
         <v>1</v>
       </c>
       <c r="G263" t="n">
-        <v>0.1373626374</v>
+        <v>0.1360544218</v>
       </c>
       <c r="H263" t="n">
         <v>0</v>
@@ -26491,25 +26075,25 @@
     </row>
     <row r="264">
       <c r="A264" s="1" t="n">
-        <v>44027</v>
+        <v>44028</v>
       </c>
       <c r="B264" t="s">
         <v>20</v>
       </c>
       <c r="C264" t="n">
-        <v>5441</v>
+        <v>5556</v>
       </c>
       <c r="D264" t="n">
-        <v>20.710261876</v>
+        <v>20.623608018</v>
       </c>
       <c r="E264" t="n">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F264" t="n">
         <v>93</v>
       </c>
       <c r="G264" t="n">
-        <v>12.774725275</v>
+        <v>12.653061224</v>
       </c>
       <c r="H264" t="n">
         <v>0</v>
@@ -26517,184 +26101,28 @@
     </row>
     <row r="265">
       <c r="A265" s="1" t="n">
-        <v>44027</v>
+        <v>44028</v>
       </c>
       <c r="B265" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C265" t="n">
-        <v>5441</v>
+        <v>6641</v>
       </c>
       <c r="D265" t="n">
-        <v>20.710261876</v>
+        <v>24.651076466</v>
       </c>
       <c r="E265" t="n">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="F265" t="n">
-        <v>93</v>
+        <v>317</v>
       </c>
       <c r="G265" t="n">
-        <v>12.774725275</v>
+        <v>43.129251701</v>
       </c>
       <c r="H265" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="266">
-      <c r="A266" s="1" t="n">
-        <v>44027</v>
-      </c>
-      <c r="B266" t="s">
-        <v>20</v>
-      </c>
-      <c r="C266" t="n">
-        <v>5441</v>
-      </c>
-      <c r="D266" t="n">
-        <v>20.710261876</v>
-      </c>
-      <c r="E266" t="n">
-        <v>0</v>
-      </c>
-      <c r="F266" t="n">
-        <v>93</v>
-      </c>
-      <c r="G266" t="n">
-        <v>12.774725275</v>
-      </c>
-      <c r="H266" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="267">
-      <c r="A267" s="1" t="n">
-        <v>44027</v>
-      </c>
-      <c r="B267" t="s">
-        <v>20</v>
-      </c>
-      <c r="C267" t="n">
-        <v>5441</v>
-      </c>
-      <c r="D267" t="n">
-        <v>20.710261876</v>
-      </c>
-      <c r="E267" t="n">
-        <v>0</v>
-      </c>
-      <c r="F267" t="n">
-        <v>93</v>
-      </c>
-      <c r="G267" t="n">
-        <v>12.774725275</v>
-      </c>
-      <c r="H267" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="268">
-      <c r="A268" s="1" t="n">
-        <v>44027</v>
-      </c>
-      <c r="B268" t="s">
-        <v>27</v>
-      </c>
-      <c r="C268" t="n">
-        <v>6522</v>
-      </c>
-      <c r="D268" t="n">
-        <v>24.824908648</v>
-      </c>
-      <c r="E268" t="n">
-        <v>183</v>
-      </c>
-      <c r="F268" t="n">
-        <v>315</v>
-      </c>
-      <c r="G268" t="n">
-        <v>43.269230769</v>
-      </c>
-      <c r="H268" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="269">
-      <c r="A269" s="1" t="n">
-        <v>44027</v>
-      </c>
-      <c r="B269" t="s">
-        <v>27</v>
-      </c>
-      <c r="C269" t="n">
-        <v>6522</v>
-      </c>
-      <c r="D269" t="n">
-        <v>24.824908648</v>
-      </c>
-      <c r="E269" t="n">
-        <v>183</v>
-      </c>
-      <c r="F269" t="n">
-        <v>315</v>
-      </c>
-      <c r="G269" t="n">
-        <v>43.269230769</v>
-      </c>
-      <c r="H269" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="270">
-      <c r="A270" s="1" t="n">
-        <v>44027</v>
-      </c>
-      <c r="B270" t="s">
-        <v>27</v>
-      </c>
-      <c r="C270" t="n">
-        <v>6522</v>
-      </c>
-      <c r="D270" t="n">
-        <v>24.824908648</v>
-      </c>
-      <c r="E270" t="n">
-        <v>0</v>
-      </c>
-      <c r="F270" t="n">
-        <v>315</v>
-      </c>
-      <c r="G270" t="n">
-        <v>43.269230769</v>
-      </c>
-      <c r="H270" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="271">
-      <c r="A271" s="1" t="n">
-        <v>44027</v>
-      </c>
-      <c r="B271" t="s">
-        <v>27</v>
-      </c>
-      <c r="C271" t="n">
-        <v>6522</v>
-      </c>
-      <c r="D271" t="n">
-        <v>24.824908648</v>
-      </c>
-      <c r="E271" t="n">
-        <v>0</v>
-      </c>
-      <c r="F271" t="n">
-        <v>315</v>
-      </c>
-      <c r="G271" t="n">
-        <v>43.269230769</v>
-      </c>
-      <c r="H271" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>